<commit_message>
Updated getWatershed to use IEc file, updated tablesOut and tablesToExcel to reflect the change from Upper and Lower Mortendad.
</commit_message>
<xml_diff>
--- a/Tables/Alluvial.xlsx
+++ b/Tables/Alluvial.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1045,12 +1045,12 @@
       </c>
       <c r="V5" s="1" t="inlineStr">
         <is>
-          <t>8.15</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="W5" s="1" t="inlineStr">
         <is>
-          <t>2013-03-28</t>
+          <t>2014-08-01</t>
         </is>
       </c>
       <c r="X5" s="1" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="AD5" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AE5" s="1" t="inlineStr">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="AG5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Substantial
 </t>
         </is>
       </c>
@@ -1173,12 +1173,12 @@
       </c>
       <c r="V6" s="1" t="inlineStr">
         <is>
-          <t>9.43</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="W6" s="1" t="inlineStr">
         <is>
-          <t>2013-03-29</t>
+          <t>2014-08-04</t>
         </is>
       </c>
       <c r="X6" s="1" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="AD6" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AE6" s="1" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="AG6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Substantial
 </t>
         </is>
       </c>
@@ -1236,7 +1236,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>SWA-2-4</t>
+          <t>SWA-3-7</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -1246,110 +1246,126 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>35.8745609</t>
+          <t>35.87376</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>-106.3125236</t>
+          <t>-106.31114</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr"/>
-      <c r="G7" s="1" t="inlineStr"/>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>2016-06-27 00:00:00</t>
+        </is>
+      </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>2 in</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr">
         <is>
-          <t>Formerly SCPZ-4, Formerly SCPZ-4, Formerly SCPZ-4</t>
-        </is>
-      </c>
-      <c r="M7" s="1" t="inlineStr">
-        <is>
-          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12447</t>
-        </is>
-      </c>
-      <c r="N7" s="1" t="inlineStr"/>
-      <c r="O7" s="1" t="inlineStr"/>
+          <t>Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7</t>
+        </is>
+      </c>
+      <c r="M7" s="1" t="inlineStr"/>
+      <c r="N7" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="O7" s="1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
       <c r="P7" s="1" t="inlineStr">
         <is>
           <t>Sandia</t>
         </is>
       </c>
-      <c r="Q7" s="1" t="inlineStr"/>
+      <c r="Q7" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="R7" s="1" t="inlineStr"/>
       <c r="S7" s="1" t="inlineStr">
         <is>
-          <t>7226.48</t>
-        </is>
-      </c>
-      <c r="T7" s="1" t="inlineStr"/>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T7" s="1" t="inlineStr">
+        <is>
+          <t>Aquifer updated from MW</t>
+        </is>
+      </c>
       <c r="U7" s="1" t="inlineStr">
         <is>
-          <t>Monitoring Wells</t>
+          <t>Well Info</t>
         </is>
       </c>
       <c r="V7" s="1" t="inlineStr">
         <is>
-          <t>16.9</t>
+          <t>34.3</t>
         </is>
       </c>
       <c r="W7" s="1" t="inlineStr">
         <is>
-          <t>2017-08-15</t>
+          <t>2017-08-16</t>
         </is>
       </c>
       <c r="X7" s="1" t="inlineStr">
         <is>
-          <t>10.8</t>
+          <t>18.2</t>
         </is>
       </c>
       <c r="Y7" s="1" t="inlineStr">
         <is>
-          <t>2019-10-24</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="Z7" s="1" t="inlineStr">
         <is>
-          <t>0.641</t>
+          <t>0.508</t>
         </is>
       </c>
       <c r="AA7" s="1" t="inlineStr">
         <is>
-          <t>2017-08-15</t>
+          <t>2017-08-16</t>
         </is>
       </c>
       <c r="AB7" s="1" t="inlineStr">
         <is>
-          <t>0.265</t>
+          <t>0.186</t>
         </is>
       </c>
       <c r="AC7" s="1" t="inlineStr">
         <is>
-          <t>2019-10-24</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="AD7" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="AE7" s="1" t="inlineStr">
@@ -1372,7 +1388,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>SWA-2-5</t>
+          <t>SWA-3-8</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1382,80 +1398,96 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>35.874674</t>
+          <t>35.8738</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>-106.3124817</t>
+          <t>-106.31109</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr"/>
-      <c r="G8" s="1" t="inlineStr"/>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>2016-06-27 00:00:00</t>
+        </is>
+      </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
-          <t>8.96</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>2 in</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr">
         <is>
-          <t>8.96</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="L8" s="1" t="inlineStr">
         <is>
-          <t>Formerly SCPZ-5, Formerly SCPZ-5, Formerly SCPZ-5</t>
-        </is>
-      </c>
-      <c r="M8" s="1" t="inlineStr">
-        <is>
-          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12448</t>
-        </is>
-      </c>
-      <c r="N8" s="1" t="inlineStr"/>
-      <c r="O8" s="1" t="inlineStr"/>
+          <t>Formerly SWA-3, Formerly SWA-3, Formerly SWA-3, Formerly SWA-3</t>
+        </is>
+      </c>
+      <c r="M8" s="1" t="inlineStr"/>
+      <c r="N8" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="O8" s="1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
       <c r="P8" s="1" t="inlineStr">
         <is>
           <t>Sandia</t>
         </is>
       </c>
-      <c r="Q8" s="1" t="inlineStr"/>
+      <c r="Q8" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="R8" s="1" t="inlineStr"/>
       <c r="S8" s="1" t="inlineStr">
         <is>
-          <t>7226.22</t>
-        </is>
-      </c>
-      <c r="T8" s="1" t="inlineStr"/>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T8" s="1" t="inlineStr">
+        <is>
+          <t>Aquifer updated from MW</t>
+        </is>
+      </c>
       <c r="U8" s="1" t="inlineStr">
         <is>
-          <t>Monitoring Wells</t>
+          <t>Well Info</t>
         </is>
       </c>
       <c r="V8" s="1" t="inlineStr">
         <is>
-          <t>8.28</t>
+          <t>22.0</t>
         </is>
       </c>
       <c r="W8" s="1" t="inlineStr">
         <is>
-          <t>2018-02-28</t>
+          <t>2018-05-31</t>
         </is>
       </c>
       <c r="X8" s="1" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>14.1</t>
         </is>
       </c>
       <c r="Y8" s="1" t="inlineStr">
@@ -1465,17 +1497,17 @@
       </c>
       <c r="Z8" s="1" t="inlineStr">
         <is>
-          <t>0.366</t>
+          <t>1.22</t>
         </is>
       </c>
       <c r="AA8" s="1" t="inlineStr">
         <is>
-          <t>2017-08-15</t>
+          <t>2017-11-30</t>
         </is>
       </c>
       <c r="AB8" s="1" t="inlineStr">
         <is>
-          <t>0.358</t>
+          <t>0.473</t>
         </is>
       </c>
       <c r="AC8" s="1" t="inlineStr">
@@ -1508,7 +1540,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>SWA-2-6</t>
+          <t>SWA-3-9</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
@@ -1518,110 +1550,126 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>35.8747486</t>
+          <t>35.87386</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>-106.3124341</t>
+          <t>-106.31105</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr"/>
-      <c r="G9" s="1" t="inlineStr"/>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t>2016-07-05 00:00:00</t>
+        </is>
+      </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
-          <t>8.22</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>2 in</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>3.12</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>8.22</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="L9" s="1" t="inlineStr">
         <is>
-          <t>Formerly SWA-2, Formerly SWA-2, Formerly SWA-2</t>
-        </is>
-      </c>
-      <c r="M9" s="1" t="inlineStr">
-        <is>
-          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12449</t>
-        </is>
-      </c>
-      <c r="N9" s="1" t="inlineStr"/>
-      <c r="O9" s="1" t="inlineStr"/>
+          <t>Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9</t>
+        </is>
+      </c>
+      <c r="M9" s="1" t="inlineStr"/>
+      <c r="N9" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="O9" s="1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
       <c r="P9" s="1" t="inlineStr">
         <is>
           <t>Sandia</t>
         </is>
       </c>
-      <c r="Q9" s="1" t="inlineStr"/>
+      <c r="Q9" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="R9" s="1" t="inlineStr"/>
       <c r="S9" s="1" t="inlineStr">
         <is>
-          <t>7225.72</t>
-        </is>
-      </c>
-      <c r="T9" s="1" t="inlineStr"/>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T9" s="1" t="inlineStr">
+        <is>
+          <t>Aquifer updated from MW</t>
+        </is>
+      </c>
       <c r="U9" s="1" t="inlineStr">
         <is>
-          <t>Monitoring Wells</t>
+          <t>Well Info</t>
         </is>
       </c>
       <c r="V9" s="1" t="inlineStr">
         <is>
-          <t>7.38</t>
+          <t>15.9</t>
         </is>
       </c>
       <c r="W9" s="1" t="inlineStr">
         <is>
-          <t>2018-02-28</t>
+          <t>2018-07-25</t>
         </is>
       </c>
       <c r="X9" s="1" t="inlineStr">
         <is>
-          <t>3.85</t>
+          <t>9.02</t>
         </is>
       </c>
       <c r="Y9" s="1" t="inlineStr">
         <is>
-          <t>2019-10-24</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="Z9" s="1" t="inlineStr">
         <is>
-          <t>0.384</t>
+          <t>0.317</t>
         </is>
       </c>
       <c r="AA9" s="1" t="inlineStr">
         <is>
+          <t>2017-08-16</t>
+        </is>
+      </c>
+      <c r="AB9" s="1" t="inlineStr">
+        <is>
+          <t>0.174</t>
+        </is>
+      </c>
+      <c r="AC9" s="1" t="inlineStr">
+        <is>
           <t>2019-02-27</t>
         </is>
       </c>
-      <c r="AB9" s="1" t="inlineStr">
-        <is>
-          <t>0.152</t>
-        </is>
-      </c>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>2019-10-24</t>
-        </is>
-      </c>
       <c r="AD9" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="AE9" s="1" t="inlineStr">
@@ -1629,7 +1677,11 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF9" s="1" t="inlineStr"/>
+      <c r="AF9" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
       <c r="AG9" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -1640,7 +1692,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-7</t>
+          <t>MCO-0.6</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
@@ -1650,24 +1702,32 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>35.87376</t>
+          <t>35.86789</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>-106.31114</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="inlineStr"/>
-      <c r="F10" s="1" t="inlineStr"/>
+          <t>-106.30545</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>7188.280</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>2016-06-27 00:00:00</t>
+          <t>1999-02-25 00:00:00</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.10</t>
         </is>
       </c>
       <c r="I10" s="1" t="inlineStr">
@@ -1677,19 +1737,15 @@
       </c>
       <c r="J10" s="1" t="inlineStr">
         <is>
-          <t>0.6</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="K10" s="1" t="inlineStr">
         <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="L10" s="1" t="inlineStr">
-        <is>
-          <t>Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7</t>
-        </is>
-      </c>
+          <t>3.050</t>
+        </is>
+      </c>
+      <c r="L10" s="1" t="inlineStr"/>
       <c r="M10" s="1" t="inlineStr"/>
       <c r="N10" s="1" t="inlineStr">
         <is>
@@ -1703,7 +1759,7 @@
       </c>
       <c r="P10" s="1" t="inlineStr">
         <is>
-          <t>Sandia</t>
+          <t>Mortendad</t>
         </is>
       </c>
       <c r="Q10" s="1" t="inlineStr">
@@ -1717,11 +1773,7 @@
           <t>[84]</t>
         </is>
       </c>
-      <c r="T10" s="1" t="inlineStr">
-        <is>
-          <t>Aquifer updated from MW</t>
-        </is>
-      </c>
+      <c r="T10" s="1" t="inlineStr"/>
       <c r="U10" s="1" t="inlineStr">
         <is>
           <t>Well Info</t>
@@ -1729,47 +1781,47 @@
       </c>
       <c r="V10" s="1" t="inlineStr">
         <is>
-          <t>34.3</t>
+          <t>662.0</t>
         </is>
       </c>
       <c r="W10" s="1" t="inlineStr">
         <is>
-          <t>2017-08-16</t>
+          <t>2010-07-02</t>
         </is>
       </c>
       <c r="X10" s="1" t="inlineStr">
         <is>
-          <t>18.2</t>
+          <t>3.09</t>
         </is>
       </c>
       <c r="Y10" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>2016-05-19</t>
         </is>
       </c>
       <c r="Z10" s="1" t="inlineStr">
         <is>
-          <t>0.508</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AA10" s="1" t="inlineStr">
         <is>
-          <t>2017-08-16</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AB10" s="1" t="inlineStr">
         <is>
-          <t>0.186</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AC10" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AD10" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>25</t>
         </is>
       </c>
       <c r="AE10" s="1" t="inlineStr">
@@ -1792,7 +1844,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-8</t>
+          <t>MCO-5</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
@@ -1802,60 +1854,60 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>35.8738</t>
+          <t>35.86339</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>-106.31109</t>
-        </is>
-      </c>
-      <c r="E11" s="1" t="inlineStr"/>
-      <c r="F11" s="1" t="inlineStr"/>
+          <t>-106.27683</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr">
+        <is>
+          <t>6875.66</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>2016-06-27 00:00:00</t>
+          <t>1960-10-01 00:00:00</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>46.00</t>
         </is>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>21</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr">
         <is>
-          <t>7.8</t>
-        </is>
-      </c>
-      <c r="L11" s="1" t="inlineStr">
-        <is>
-          <t>Formerly SWA-3, Formerly SWA-3, Formerly SWA-3, Formerly SWA-3</t>
-        </is>
-      </c>
+          <t>46.000</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr"/>
       <c r="M11" s="1" t="inlineStr"/>
-      <c r="N11" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
+      <c r="N11" s="1" t="inlineStr"/>
       <c r="O11" s="1" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Chromium</t>
         </is>
       </c>
       <c r="P11" s="1" t="inlineStr">
         <is>
-          <t>Sandia</t>
+          <t>Mortendad</t>
         </is>
       </c>
       <c r="Q11" s="1" t="inlineStr">
@@ -1871,7 +1923,7 @@
       </c>
       <c r="T11" s="1" t="inlineStr">
         <is>
-          <t>Aquifer updated from MW</t>
+          <t>Ground Elevation updated from MW</t>
         </is>
       </c>
       <c r="U11" s="1" t="inlineStr">
@@ -1881,47 +1933,47 @@
       </c>
       <c r="V11" s="1" t="inlineStr">
         <is>
-          <t>22.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="W11" s="1" t="inlineStr">
         <is>
-          <t>2018-05-31</t>
+          <t>2008-02-07</t>
         </is>
       </c>
       <c r="X11" s="1" t="inlineStr">
         <is>
-          <t>14.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y11" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>2019-07-22</t>
         </is>
       </c>
       <c r="Z11" s="1" t="inlineStr">
         <is>
-          <t>1.22</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AA11" s="1" t="inlineStr">
         <is>
-          <t>2017-11-30</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AB11" s="1" t="inlineStr">
         <is>
-          <t>0.473</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AC11" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AD11" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>49</t>
         </is>
       </c>
       <c r="AE11" s="1" t="inlineStr">
@@ -1929,11 +1981,7 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF11" s="1" t="inlineStr">
-        <is>
-          <t>Exceedance</t>
-        </is>
-      </c>
+      <c r="AF11" s="1" t="inlineStr"/>
       <c r="AG11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -1944,7 +1992,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-9</t>
+          <t>MCO-7</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
@@ -1954,60 +2002,60 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>35.87386</t>
+          <t>35.86056</t>
         </is>
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>-106.31105</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="inlineStr"/>
-      <c r="F12" s="1" t="inlineStr"/>
+          <t>-106.26991</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>6827.31</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>2016-07-05 00:00:00</t>
+          <t>1960-10-01 00:00:00</t>
         </is>
       </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>69.00</t>
         </is>
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J12" s="1" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>39</t>
         </is>
       </c>
       <c r="K12" s="1" t="inlineStr">
         <is>
-          <t>4.7</t>
-        </is>
-      </c>
-      <c r="L12" s="1" t="inlineStr">
-        <is>
-          <t>Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9</t>
-        </is>
-      </c>
+          <t>69.000</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr"/>
       <c r="M12" s="1" t="inlineStr"/>
-      <c r="N12" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
+      <c r="N12" s="1" t="inlineStr"/>
       <c r="O12" s="1" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Chromium</t>
         </is>
       </c>
       <c r="P12" s="1" t="inlineStr">
         <is>
-          <t>Sandia</t>
+          <t>Mortendad</t>
         </is>
       </c>
       <c r="Q12" s="1" t="inlineStr">
@@ -2023,7 +2071,7 @@
       </c>
       <c r="T12" s="1" t="inlineStr">
         <is>
-          <t>Aquifer updated from MW</t>
+          <t>Ground Elevation updated from MW</t>
         </is>
       </c>
       <c r="U12" s="1" t="inlineStr">
@@ -2033,47 +2081,47 @@
       </c>
       <c r="V12" s="1" t="inlineStr">
         <is>
-          <t>15.9</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="W12" s="1" t="inlineStr">
         <is>
-          <t>2018-07-25</t>
+          <t>2008-02-25</t>
         </is>
       </c>
       <c r="X12" s="1" t="inlineStr">
         <is>
-          <t>9.02</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y12" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>2019-07-22</t>
         </is>
       </c>
       <c r="Z12" s="1" t="inlineStr">
         <is>
-          <t>0.317</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AA12" s="1" t="inlineStr">
         <is>
-          <t>2017-08-16</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AB12" s="1" t="inlineStr">
         <is>
-          <t>0.174</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AC12" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AD12" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>48</t>
         </is>
       </c>
       <c r="AE12" s="1" t="inlineStr">
@@ -2081,11 +2129,7 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF12" s="1" t="inlineStr">
-        <is>
-          <t>Exceedance</t>
-        </is>
-      </c>
+      <c r="AF12" s="1" t="inlineStr"/>
       <c r="AG12" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -2096,7 +2140,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>SWA-4-10</t>
+          <t>LAO-3a</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
@@ -2106,110 +2150,130 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>35.8735723</t>
+          <t>35.87317</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>-106.3106197</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="inlineStr"/>
-      <c r="F13" s="1" t="inlineStr"/>
-      <c r="G13" s="1" t="inlineStr"/>
+          <t>-106.25822</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>6609.1</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="inlineStr">
+        <is>
+          <t>1989-09-14 00:00:00</t>
+        </is>
+      </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>8.44</t>
+          <t>14.70</t>
         </is>
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>2 in</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr">
         <is>
-          <t>8.44</t>
+          <t>14.700</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
         <is>
-          <t>Formerly SCPZ-10, Formerly SCPZ-10, Formerly SCPZ-10</t>
-        </is>
-      </c>
-      <c r="M13" s="1" t="inlineStr">
-        <is>
-          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12453</t>
-        </is>
-      </c>
+          <t>Elevation revised based on LIDAR surface location pick, Elevation revised based on LIDAR surface location pick</t>
+        </is>
+      </c>
+      <c r="M13" s="1" t="inlineStr"/>
       <c r="N13" s="1" t="inlineStr"/>
-      <c r="O13" s="1" t="inlineStr"/>
+      <c r="O13" s="1" t="inlineStr">
+        <is>
+          <t>TA-21</t>
+        </is>
+      </c>
       <c r="P13" s="1" t="inlineStr">
         <is>
-          <t>Sandia</t>
-        </is>
-      </c>
-      <c r="Q13" s="1" t="inlineStr"/>
+          <t>Los Alamos</t>
+        </is>
+      </c>
+      <c r="Q13" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="R13" s="1" t="inlineStr"/>
       <c r="S13" s="1" t="inlineStr">
         <is>
-          <t>7213.06</t>
-        </is>
-      </c>
-      <c r="T13" s="1" t="inlineStr"/>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T13" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
       <c r="U13" s="1" t="inlineStr">
         <is>
-          <t>Monitoring Wells</t>
+          <t>Well Info</t>
         </is>
       </c>
       <c r="V13" s="1" t="inlineStr">
         <is>
-          <t>72.0</t>
+          <t>13.9</t>
         </is>
       </c>
       <c r="W13" s="1" t="inlineStr">
         <is>
-          <t>2018-07-25</t>
+          <t>2003-09-17</t>
         </is>
       </c>
       <c r="X13" s="1" t="inlineStr">
         <is>
-          <t>36.5</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y13" s="1" t="inlineStr">
         <is>
-          <t>2019-10-23</t>
+          <t>2019-06-25</t>
         </is>
       </c>
       <c r="Z13" s="1" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AA13" s="1" t="inlineStr">
         <is>
-          <t>2017-05-23</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AB13" s="1" t="inlineStr">
         <is>
-          <t>0.584</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AC13" s="1" t="inlineStr">
         <is>
-          <t>2019-10-23</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AD13" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>35</t>
         </is>
       </c>
       <c r="AE13" s="1" t="inlineStr">
@@ -2232,7 +2296,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>SWA-4-11</t>
+          <t>LAUZ-1</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -2242,110 +2306,122 @@
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>35.8736526</t>
+          <t>35.87787</t>
         </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>-106.3105976</t>
-        </is>
-      </c>
-      <c r="E14" s="1" t="inlineStr"/>
+          <t>-106.27357</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr">
+        <is>
+          <t>7032.42</t>
+        </is>
+      </c>
       <c r="F14" s="1" t="inlineStr"/>
       <c r="G14" s="1" t="inlineStr"/>
       <c r="H14" s="1" t="inlineStr">
         <is>
-          <t>9.17</t>
+          <t>10.55</t>
         </is>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>2 in</t>
+          <t>4 in</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5.35</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
         <is>
-          <t>9.17</t>
+          <t>10.350</t>
         </is>
       </c>
       <c r="L14" s="1" t="inlineStr">
         <is>
-          <t>Formerly SCPZ-11(B), Formerly SCPZ-11(B), Formerly SCPZ-11(B)</t>
-        </is>
-      </c>
-      <c r="M14" s="1" t="inlineStr">
-        <is>
-          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12454</t>
-        </is>
-      </c>
+          <t>DP Canyon, OU 1106 (TA-21), Surv-Tek Survey, Surv-Tek Survey</t>
+        </is>
+      </c>
+      <c r="M14" s="1" t="inlineStr"/>
       <c r="N14" s="1" t="inlineStr"/>
-      <c r="O14" s="1" t="inlineStr"/>
+      <c r="O14" s="1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
       <c r="P14" s="1" t="inlineStr">
         <is>
-          <t>Sandia</t>
-        </is>
-      </c>
-      <c r="Q14" s="1" t="inlineStr"/>
+          <t>Los Alamos</t>
+        </is>
+      </c>
+      <c r="Q14" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="R14" s="1" t="inlineStr"/>
       <c r="S14" s="1" t="inlineStr">
         <is>
-          <t>7214.07</t>
-        </is>
-      </c>
-      <c r="T14" s="1" t="inlineStr"/>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T14" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW, Well Diameter [in] updated from MW</t>
+        </is>
+      </c>
       <c r="U14" s="1" t="inlineStr">
         <is>
-          <t>Monitoring Wells</t>
+          <t>Well Info</t>
         </is>
       </c>
       <c r="V14" s="1" t="inlineStr">
         <is>
-          <t>44.4</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="W14" s="1" t="inlineStr">
         <is>
-          <t>2017-08-15</t>
+          <t>1997-08-20</t>
         </is>
       </c>
       <c r="X14" s="1" t="inlineStr">
         <is>
-          <t>14.5</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y14" s="1" t="inlineStr">
         <is>
-          <t>2019-10-23</t>
+          <t>2019-06-19</t>
         </is>
       </c>
       <c r="Z14" s="1" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AA14" s="1" t="inlineStr">
         <is>
-          <t>2017-05-23</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AB14" s="1" t="inlineStr">
         <is>
-          <t>0.328</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AC14" s="1" t="inlineStr">
         <is>
-          <t>2019-10-23</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AD14" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>32</t>
         </is>
       </c>
       <c r="AE14" s="1" t="inlineStr">
@@ -2353,11 +2429,7 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF14" s="1" t="inlineStr">
-        <is>
-          <t>Exceedance</t>
-        </is>
-      </c>
+      <c r="AF14" s="1" t="inlineStr"/>
       <c r="AG14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -2368,7 +2440,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>SWA-4-12</t>
+          <t>PAO-5n</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
@@ -2378,110 +2450,126 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>35.8737001</t>
+          <t>35.87326</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>-106.3105616</t>
-        </is>
-      </c>
-      <c r="E15" s="1" t="inlineStr"/>
-      <c r="F15" s="1" t="inlineStr"/>
-      <c r="G15" s="1" t="inlineStr"/>
+          <t>-106.22011</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="inlineStr">
+        <is>
+          <t>6369.79</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
+      <c r="G15" s="1" t="inlineStr">
+        <is>
+          <t>1998-03-24 00:00:00</t>
+        </is>
+      </c>
       <c r="H15" s="1" t="inlineStr">
         <is>
-          <t>8.53</t>
+          <t>15.28</t>
         </is>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>2 in</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>2.99</t>
+          <t>7.43</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
         <is>
-          <t>8.19</t>
-        </is>
-      </c>
-      <c r="L15" s="1" t="inlineStr">
-        <is>
-          <t>Formerly SWA-4, Formerly SWA-4, Formerly SWA-4</t>
-        </is>
-      </c>
-      <c r="M15" s="1" t="inlineStr">
-        <is>
-          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12455</t>
-        </is>
-      </c>
+          <t>12.430</t>
+        </is>
+      </c>
+      <c r="L15" s="1" t="inlineStr"/>
+      <c r="M15" s="1" t="inlineStr"/>
       <c r="N15" s="1" t="inlineStr"/>
-      <c r="O15" s="1" t="inlineStr"/>
+      <c r="O15" s="1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
       <c r="P15" s="1" t="inlineStr">
         <is>
-          <t>Sandia</t>
-        </is>
-      </c>
-      <c r="Q15" s="1" t="inlineStr"/>
+          <t>Los Alamos</t>
+        </is>
+      </c>
+      <c r="Q15" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="R15" s="1" t="inlineStr"/>
       <c r="S15" s="1" t="inlineStr">
         <is>
-          <t>7213.04</t>
-        </is>
-      </c>
-      <c r="T15" s="1" t="inlineStr"/>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T15" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
       <c r="U15" s="1" t="inlineStr">
         <is>
-          <t>Monitoring Wells</t>
+          <t>Well Info</t>
         </is>
       </c>
       <c r="V15" s="1" t="inlineStr">
         <is>
-          <t>56.2</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="W15" s="1" t="inlineStr">
         <is>
-          <t>2017-08-15</t>
+          <t>2015-06-04</t>
         </is>
       </c>
       <c r="X15" s="1" t="inlineStr">
         <is>
-          <t>31.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y15" s="1" t="inlineStr">
         <is>
-          <t>2019-10-23</t>
+          <t>2019-06-20</t>
         </is>
       </c>
       <c r="Z15" s="1" t="inlineStr">
         <is>
-          <t>1.74</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AA15" s="1" t="inlineStr">
         <is>
-          <t>2017-05-23</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AB15" s="1" t="inlineStr">
         <is>
-          <t>0.693</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AC15" s="1" t="inlineStr">
         <is>
-          <t>2019-10-23</t>
+          <t>No Data</t>
         </is>
       </c>
       <c r="AD15" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="AE15" s="1" t="inlineStr">
@@ -2489,11 +2577,7 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF15" s="1" t="inlineStr">
-        <is>
-          <t>Exceedance</t>
-        </is>
-      </c>
+      <c r="AF15" s="1" t="inlineStr"/>
       <c r="AG15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -2504,7 +2588,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>MCO-0.6</t>
+          <t>18-MW-18</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
@@ -2514,17 +2598,17 @@
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>35.86789</t>
+          <t>35.83237</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>-106.30545</t>
+          <t>-106.25166</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>7188.280</t>
+          <t>6654.7</t>
         </is>
       </c>
       <c r="F16" s="1" t="inlineStr">
@@ -2534,12 +2618,12 @@
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>1999-02-25 00:00:00</t>
+          <t>1995-07-31 00:00:00</t>
         </is>
       </c>
       <c r="H16" s="1" t="inlineStr">
         <is>
-          <t>3.10</t>
+          <t>23.00</t>
         </is>
       </c>
       <c r="I16" s="1" t="inlineStr">
@@ -2549,29 +2633,29 @@
       </c>
       <c r="J16" s="1" t="inlineStr">
         <is>
-          <t>1.05</t>
+          <t>12.5</t>
         </is>
       </c>
       <c r="K16" s="1" t="inlineStr">
         <is>
-          <t>3.050</t>
-        </is>
-      </c>
-      <c r="L16" s="1" t="inlineStr"/>
+          <t>23.000</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>TA-18</t>
+        </is>
+      </c>
       <c r="M16" s="1" t="inlineStr"/>
-      <c r="N16" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
+      <c r="N16" s="1" t="inlineStr"/>
       <c r="O16" s="1" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>TA-54</t>
         </is>
       </c>
       <c r="P16" s="1" t="inlineStr">
         <is>
-          <t>Upper Mortendad</t>
+          <t>Pajarito</t>
         </is>
       </c>
       <c r="Q16" s="1" t="inlineStr">
@@ -2585,7 +2669,11 @@
           <t>[84]</t>
         </is>
       </c>
-      <c r="T16" s="1" t="inlineStr"/>
+      <c r="T16" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
       <c r="U16" s="1" t="inlineStr">
         <is>
           <t>Well Info</t>
@@ -2593,22 +2681,22 @@
       </c>
       <c r="V16" s="1" t="inlineStr">
         <is>
-          <t>662.0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="W16" s="1" t="inlineStr">
         <is>
-          <t>2010-07-02</t>
+          <t>2007-03-19</t>
         </is>
       </c>
       <c r="X16" s="1" t="inlineStr">
         <is>
-          <t>3.09</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y16" s="1" t="inlineStr">
         <is>
-          <t>2016-05-19</t>
+          <t>2019-10-31</t>
         </is>
       </c>
       <c r="Z16" s="1" t="inlineStr">
@@ -2633,7 +2721,7 @@
       </c>
       <c r="AD16" s="1" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>38</t>
         </is>
       </c>
       <c r="AE16" s="1" t="inlineStr">
@@ -2656,7 +2744,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>MCO-5</t>
+          <t>PCAO-8</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
@@ -2666,17 +2754,17 @@
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>35.86339</t>
+          <t>35.82722</t>
         </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>-106.27683</t>
+          <t>-106.23837</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>6875.66</t>
+          <t>6584.450</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
@@ -2686,40 +2774,48 @@
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>1960-10-01 00:00:00</t>
+          <t>2008-06-02 00:00:00</t>
         </is>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
-          <t>46.00</t>
+          <t>25.00</t>
         </is>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
         <is>
-          <t>46.000</t>
-        </is>
-      </c>
-      <c r="L17" s="1" t="inlineStr"/>
+          <t>19.700</t>
+        </is>
+      </c>
+      <c r="L17" s="1" t="inlineStr">
+        <is>
+          <t>Brass Cap, Brass Cap, Brass Cap</t>
+        </is>
+      </c>
       <c r="M17" s="1" t="inlineStr"/>
-      <c r="N17" s="1" t="inlineStr"/>
+      <c r="N17" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
       <c r="O17" s="1" t="inlineStr">
         <is>
-          <t>Chromium</t>
+          <t>TA-54</t>
         </is>
       </c>
       <c r="P17" s="1" t="inlineStr">
         <is>
-          <t>Lower Mortendad</t>
+          <t>Pajarito</t>
         </is>
       </c>
       <c r="Q17" s="1" t="inlineStr">
@@ -2733,11 +2829,7 @@
           <t>[84]</t>
         </is>
       </c>
-      <c r="T17" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
+      <c r="T17" s="1" t="inlineStr"/>
       <c r="U17" s="1" t="inlineStr">
         <is>
           <t>Well Info</t>
@@ -2745,12 +2837,12 @@
       </c>
       <c r="V17" s="1" t="inlineStr">
         <is>
-          <t>5.76</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="W17" s="1" t="inlineStr">
         <is>
-          <t>2010-07-06</t>
+          <t>2008-06-24</t>
         </is>
       </c>
       <c r="X17" s="1" t="inlineStr">
@@ -2760,7 +2852,7 @@
       </c>
       <c r="Y17" s="1" t="inlineStr">
         <is>
-          <t>2019-07-22</t>
+          <t>2019-04-17</t>
         </is>
       </c>
       <c r="Z17" s="1" t="inlineStr">
@@ -2785,7 +2877,7 @@
       </c>
       <c r="AD17" s="1" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>12</t>
         </is>
       </c>
       <c r="AE17" s="1" t="inlineStr">
@@ -2795,910 +2887,6 @@
       </c>
       <c r="AF17" s="1" t="inlineStr"/>
       <c r="AG17" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Substantial
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>MCO-7</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>Alluvial</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>35.86056</t>
-        </is>
-      </c>
-      <c r="D18" s="1" t="inlineStr">
-        <is>
-          <t>-106.26991</t>
-        </is>
-      </c>
-      <c r="E18" s="1" t="inlineStr">
-        <is>
-          <t>6827.31</t>
-        </is>
-      </c>
-      <c r="F18" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
-      <c r="G18" s="1" t="inlineStr">
-        <is>
-          <t>1960-10-01 00:00:00</t>
-        </is>
-      </c>
-      <c r="H18" s="1" t="inlineStr">
-        <is>
-          <t>69.00</t>
-        </is>
-      </c>
-      <c r="I18" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J18" s="1" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="K18" s="1" t="inlineStr">
-        <is>
-          <t>69.000</t>
-        </is>
-      </c>
-      <c r="L18" s="1" t="inlineStr"/>
-      <c r="M18" s="1" t="inlineStr"/>
-      <c r="N18" s="1" t="inlineStr"/>
-      <c r="O18" s="1" t="inlineStr">
-        <is>
-          <t>Chromium</t>
-        </is>
-      </c>
-      <c r="P18" s="1" t="inlineStr">
-        <is>
-          <t>Lower Mortendad</t>
-        </is>
-      </c>
-      <c r="Q18" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="R18" s="1" t="inlineStr"/>
-      <c r="S18" s="1" t="inlineStr">
-        <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T18" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
-      <c r="U18" s="1" t="inlineStr">
-        <is>
-          <t>Well Info</t>
-        </is>
-      </c>
-      <c r="V18" s="1" t="inlineStr">
-        <is>
-          <t>5.44</t>
-        </is>
-      </c>
-      <c r="W18" s="1" t="inlineStr">
-        <is>
-          <t>2010-07-07</t>
-        </is>
-      </c>
-      <c r="X18" s="1" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Y18" s="1" t="inlineStr">
-        <is>
-          <t>2019-07-22</t>
-        </is>
-      </c>
-      <c r="Z18" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AA18" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AB18" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AC18" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AD18" s="1" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
-      </c>
-      <c r="AE18" s="1" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="AF18" s="1" t="inlineStr"/>
-      <c r="AG18" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Substantial
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>LAO-3a</t>
-        </is>
-      </c>
-      <c r="B19" s="1" t="inlineStr">
-        <is>
-          <t>Alluvial</t>
-        </is>
-      </c>
-      <c r="C19" s="1" t="inlineStr">
-        <is>
-          <t>35.87317</t>
-        </is>
-      </c>
-      <c r="D19" s="1" t="inlineStr">
-        <is>
-          <t>-106.25822</t>
-        </is>
-      </c>
-      <c r="E19" s="1" t="inlineStr">
-        <is>
-          <t>6609.1</t>
-        </is>
-      </c>
-      <c r="F19" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
-      <c r="G19" s="1" t="inlineStr">
-        <is>
-          <t>1989-09-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="H19" s="1" t="inlineStr">
-        <is>
-          <t>14.70</t>
-        </is>
-      </c>
-      <c r="I19" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J19" s="1" t="inlineStr">
-        <is>
-          <t>4.7</t>
-        </is>
-      </c>
-      <c r="K19" s="1" t="inlineStr">
-        <is>
-          <t>14.700</t>
-        </is>
-      </c>
-      <c r="L19" s="1" t="inlineStr">
-        <is>
-          <t>Elevation revised based on LIDAR surface location pick, Elevation revised based on LIDAR surface location pick</t>
-        </is>
-      </c>
-      <c r="M19" s="1" t="inlineStr"/>
-      <c r="N19" s="1" t="inlineStr"/>
-      <c r="O19" s="1" t="inlineStr">
-        <is>
-          <t>TA-21</t>
-        </is>
-      </c>
-      <c r="P19" s="1" t="inlineStr">
-        <is>
-          <t>Los Alamos</t>
-        </is>
-      </c>
-      <c r="Q19" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="R19" s="1" t="inlineStr"/>
-      <c r="S19" s="1" t="inlineStr">
-        <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T19" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
-      <c r="U19" s="1" t="inlineStr">
-        <is>
-          <t>Well Info</t>
-        </is>
-      </c>
-      <c r="V19" s="1" t="inlineStr">
-        <is>
-          <t>13.9</t>
-        </is>
-      </c>
-      <c r="W19" s="1" t="inlineStr">
-        <is>
-          <t>2003-09-17</t>
-        </is>
-      </c>
-      <c r="X19" s="1" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Y19" s="1" t="inlineStr">
-        <is>
-          <t>2019-06-25</t>
-        </is>
-      </c>
-      <c r="Z19" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AA19" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AB19" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AC19" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AD19" s="1" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="AE19" s="1" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="AF19" s="1" t="inlineStr">
-        <is>
-          <t>Exceedance</t>
-        </is>
-      </c>
-      <c r="AG19" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Substantial
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>LAUZ-1</t>
-        </is>
-      </c>
-      <c r="B20" s="1" t="inlineStr">
-        <is>
-          <t>Alluvial</t>
-        </is>
-      </c>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t>35.87787</t>
-        </is>
-      </c>
-      <c r="D20" s="1" t="inlineStr">
-        <is>
-          <t>-106.27357</t>
-        </is>
-      </c>
-      <c r="E20" s="1" t="inlineStr">
-        <is>
-          <t>7032.42</t>
-        </is>
-      </c>
-      <c r="F20" s="1" t="inlineStr"/>
-      <c r="G20" s="1" t="inlineStr"/>
-      <c r="H20" s="1" t="inlineStr">
-        <is>
-          <t>10.55</t>
-        </is>
-      </c>
-      <c r="I20" s="1" t="inlineStr">
-        <is>
-          <t>4 in</t>
-        </is>
-      </c>
-      <c r="J20" s="1" t="inlineStr">
-        <is>
-          <t>5.35</t>
-        </is>
-      </c>
-      <c r="K20" s="1" t="inlineStr">
-        <is>
-          <t>10.350</t>
-        </is>
-      </c>
-      <c r="L20" s="1" t="inlineStr">
-        <is>
-          <t>DP Canyon, OU 1106 (TA-21), Surv-Tek Survey, Surv-Tek Survey</t>
-        </is>
-      </c>
-      <c r="M20" s="1" t="inlineStr"/>
-      <c r="N20" s="1" t="inlineStr"/>
-      <c r="O20" s="1" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="P20" s="1" t="inlineStr">
-        <is>
-          <t>Los Alamos</t>
-        </is>
-      </c>
-      <c r="Q20" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="R20" s="1" t="inlineStr"/>
-      <c r="S20" s="1" t="inlineStr">
-        <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T20" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW, Well Diameter [in] updated from MW</t>
-        </is>
-      </c>
-      <c r="U20" s="1" t="inlineStr">
-        <is>
-          <t>Well Info</t>
-        </is>
-      </c>
-      <c r="V20" s="1" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="W20" s="1" t="inlineStr">
-        <is>
-          <t>2001-11-13</t>
-        </is>
-      </c>
-      <c r="X20" s="1" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Y20" s="1" t="inlineStr">
-        <is>
-          <t>2019-06-19</t>
-        </is>
-      </c>
-      <c r="Z20" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AA20" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AB20" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AC20" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AD20" s="1" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="AE20" s="1" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="AF20" s="1" t="inlineStr"/>
-      <c r="AG20" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Substantial
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>PAO-5n</t>
-        </is>
-      </c>
-      <c r="B21" s="1" t="inlineStr">
-        <is>
-          <t>Alluvial</t>
-        </is>
-      </c>
-      <c r="C21" s="1" t="inlineStr">
-        <is>
-          <t>35.87326</t>
-        </is>
-      </c>
-      <c r="D21" s="1" t="inlineStr">
-        <is>
-          <t>-106.22011</t>
-        </is>
-      </c>
-      <c r="E21" s="1" t="inlineStr">
-        <is>
-          <t>6369.79</t>
-        </is>
-      </c>
-      <c r="F21" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
-      <c r="G21" s="1" t="inlineStr">
-        <is>
-          <t>1998-03-24 00:00:00</t>
-        </is>
-      </c>
-      <c r="H21" s="1" t="inlineStr">
-        <is>
-          <t>15.28</t>
-        </is>
-      </c>
-      <c r="I21" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J21" s="1" t="inlineStr">
-        <is>
-          <t>7.43</t>
-        </is>
-      </c>
-      <c r="K21" s="1" t="inlineStr">
-        <is>
-          <t>12.430</t>
-        </is>
-      </c>
-      <c r="L21" s="1" t="inlineStr"/>
-      <c r="M21" s="1" t="inlineStr"/>
-      <c r="N21" s="1" t="inlineStr"/>
-      <c r="O21" s="1" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="P21" s="1" t="inlineStr">
-        <is>
-          <t>Los Alamos</t>
-        </is>
-      </c>
-      <c r="Q21" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="R21" s="1" t="inlineStr"/>
-      <c r="S21" s="1" t="inlineStr">
-        <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T21" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
-      <c r="U21" s="1" t="inlineStr">
-        <is>
-          <t>Well Info</t>
-        </is>
-      </c>
-      <c r="V21" s="1" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="W21" s="1" t="inlineStr">
-        <is>
-          <t>2002-06-11</t>
-        </is>
-      </c>
-      <c r="X21" s="1" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Y21" s="1" t="inlineStr">
-        <is>
-          <t>2019-06-20</t>
-        </is>
-      </c>
-      <c r="Z21" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AA21" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AB21" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AC21" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AD21" s="1" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="AE21" s="1" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="AF21" s="1" t="inlineStr"/>
-      <c r="AG21" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Substantial
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>18-MW-18</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t>Alluvial</t>
-        </is>
-      </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t>35.83237</t>
-        </is>
-      </c>
-      <c r="D22" s="1" t="inlineStr">
-        <is>
-          <t>-106.25166</t>
-        </is>
-      </c>
-      <c r="E22" s="1" t="inlineStr">
-        <is>
-          <t>6654.7</t>
-        </is>
-      </c>
-      <c r="F22" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
-      <c r="G22" s="1" t="inlineStr">
-        <is>
-          <t>1995-07-31 00:00:00</t>
-        </is>
-      </c>
-      <c r="H22" s="1" t="inlineStr">
-        <is>
-          <t>23.00</t>
-        </is>
-      </c>
-      <c r="I22" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J22" s="1" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="K22" s="1" t="inlineStr">
-        <is>
-          <t>23.000</t>
-        </is>
-      </c>
-      <c r="L22" s="1" t="inlineStr">
-        <is>
-          <t>TA-18</t>
-        </is>
-      </c>
-      <c r="M22" s="1" t="inlineStr"/>
-      <c r="N22" s="1" t="inlineStr"/>
-      <c r="O22" s="1" t="inlineStr">
-        <is>
-          <t>TA-54</t>
-        </is>
-      </c>
-      <c r="P22" s="1" t="inlineStr">
-        <is>
-          <t>Pajarito</t>
-        </is>
-      </c>
-      <c r="Q22" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="R22" s="1" t="inlineStr"/>
-      <c r="S22" s="1" t="inlineStr">
-        <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T22" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
-      <c r="U22" s="1" t="inlineStr">
-        <is>
-          <t>Well Info</t>
-        </is>
-      </c>
-      <c r="V22" s="1" t="inlineStr">
-        <is>
-          <t>15.0</t>
-        </is>
-      </c>
-      <c r="W22" s="1" t="inlineStr">
-        <is>
-          <t>2007-03-19</t>
-        </is>
-      </c>
-      <c r="X22" s="1" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Y22" s="1" t="inlineStr">
-        <is>
-          <t>2019-10-31</t>
-        </is>
-      </c>
-      <c r="Z22" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AA22" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AB22" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AC22" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AD22" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="AE22" s="1" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="AF22" s="1" t="inlineStr">
-        <is>
-          <t>Exceedance</t>
-        </is>
-      </c>
-      <c r="AG22" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Substantial
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>PCAO-8</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>Alluvial</t>
-        </is>
-      </c>
-      <c r="C23" s="1" t="inlineStr">
-        <is>
-          <t>35.82722</t>
-        </is>
-      </c>
-      <c r="D23" s="1" t="inlineStr">
-        <is>
-          <t>-106.23837</t>
-        </is>
-      </c>
-      <c r="E23" s="1" t="inlineStr">
-        <is>
-          <t>6584.450</t>
-        </is>
-      </c>
-      <c r="F23" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
-      <c r="G23" s="1" t="inlineStr">
-        <is>
-          <t>2008-06-02 00:00:00</t>
-        </is>
-      </c>
-      <c r="H23" s="1" t="inlineStr">
-        <is>
-          <t>25.00</t>
-        </is>
-      </c>
-      <c r="I23" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J23" s="1" t="inlineStr">
-        <is>
-          <t>9.7</t>
-        </is>
-      </c>
-      <c r="K23" s="1" t="inlineStr">
-        <is>
-          <t>19.700</t>
-        </is>
-      </c>
-      <c r="L23" s="1" t="inlineStr">
-        <is>
-          <t>Brass Cap, Brass Cap, Brass Cap</t>
-        </is>
-      </c>
-      <c r="M23" s="1" t="inlineStr"/>
-      <c r="N23" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
-      <c r="O23" s="1" t="inlineStr">
-        <is>
-          <t>TA-54</t>
-        </is>
-      </c>
-      <c r="P23" s="1" t="inlineStr">
-        <is>
-          <t>Pajarito</t>
-        </is>
-      </c>
-      <c r="Q23" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="R23" s="1" t="inlineStr"/>
-      <c r="S23" s="1" t="inlineStr">
-        <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T23" s="1" t="inlineStr"/>
-      <c r="U23" s="1" t="inlineStr">
-        <is>
-          <t>Well Info</t>
-        </is>
-      </c>
-      <c r="V23" s="1" t="inlineStr">
-        <is>
-          <t>3.01</t>
-        </is>
-      </c>
-      <c r="W23" s="1" t="inlineStr">
-        <is>
-          <t>2010-06-08</t>
-        </is>
-      </c>
-      <c r="X23" s="1" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Y23" s="1" t="inlineStr">
-        <is>
-          <t>2019-04-17</t>
-        </is>
-      </c>
-      <c r="Z23" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AA23" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AB23" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AC23" s="1" t="inlineStr">
-        <is>
-          <t>No Data</t>
-        </is>
-      </c>
-      <c r="AD23" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AE23" s="1" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="AF23" s="1" t="inlineStr"/>
-      <c r="AG23" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
 </t>
@@ -3716,7 +2904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3926,12 +3114,12 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>8.15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>3/28/13</t>
+          <t>8/1/14</t>
         </is>
       </c>
     </row>
@@ -3960,732 +3148,495 @@
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>9.43</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
-          <t>3/29/13</t>
+          <t>8/4/14</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>SWA-2-4</t>
+          <t>SWA-3-7</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>35.8745609</t>
+          <t>35.87376</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>-106.3125236</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr"/>
+          <t>-106.31114</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>6/27/16</t>
+        </is>
+      </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>3 - 9</t>
+          <t>0.6 - 3.1</t>
         </is>
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>16.9</t>
+          <t>34.3</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
-          <t>8/15/17</t>
+          <t>8/16/17</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>SWA-2-5</t>
+          <t>SWA-3-8</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>35.874674</t>
+          <t>35.8738</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>-106.3124817</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="inlineStr"/>
+          <t>-106.31109</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>6/27/16</t>
+        </is>
+      </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>8.96</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>3 - 8.96</t>
+          <t>3.6 - 7.8</t>
         </is>
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>8.28</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>2/28/18</t>
+          <t>5/31/18</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>SWA-2-6</t>
+          <t>SWA-3-9</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>35.8747486</t>
+          <t>35.87386</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>-106.3124341</t>
-        </is>
-      </c>
-      <c r="D11" s="1" t="inlineStr"/>
+          <t>-106.31105</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>7/5/16</t>
+        </is>
+      </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>8.22</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>3.12 - 8.22</t>
+          <t>2.2 - 4.7</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>7.38</t>
+          <t>15.9</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
-          <t>2/28/18</t>
+          <t>7/25/18</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>SWA-3-7</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>35.87376</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t>-106.31114</t>
-        </is>
-      </c>
-      <c r="D12" s="1" t="inlineStr">
-        <is>
-          <t>6/27/16</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="inlineStr">
-        <is>
-          <t>3.6</t>
-        </is>
-      </c>
-      <c r="F12" s="1" t="inlineStr">
-        <is>
-          <t>0.6 - 3.1</t>
-        </is>
-      </c>
-      <c r="G12" s="1" t="inlineStr">
-        <is>
-          <t>34.3</t>
-        </is>
-      </c>
-      <c r="H12" s="1" t="inlineStr">
-        <is>
-          <t>8/16/17</t>
-        </is>
-      </c>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Mortendad Canyon</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-8</t>
+          <t>MCO-0.6</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>35.8738</t>
+          <t>35.86789</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>-106.31109</t>
+          <t>-106.30545</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>6/27/16</t>
+          <t>2/25/99</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>3.6 - 7.8</t>
+          <t>1.05 - 3.05</t>
         </is>
       </c>
       <c r="G13" s="1" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>662</t>
         </is>
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>5/31/18</t>
+          <t>7/2/10</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-9</t>
+          <t>MCO-5</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>35.87386</t>
+          <t>35.86339</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>-106.31105</t>
+          <t>-106.27683</t>
         </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>7/5/16</t>
+          <t>10/1/60</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>2.2 - 4.7</t>
+          <t>21 - 46</t>
         </is>
       </c>
       <c r="G14" s="1" t="inlineStr">
         <is>
-          <t>15.9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H14" s="1" t="inlineStr">
         <is>
-          <t>7/25/18</t>
+          <t>2/7/08</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>SWA-4-10</t>
+          <t>MCO-7</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>35.8735723</t>
+          <t>35.86056</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>-106.3106197</t>
-        </is>
-      </c>
-      <c r="D15" s="1" t="inlineStr"/>
+          <t>-106.26991</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>10/1/60</t>
+        </is>
+      </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>8.44</t>
+          <t>69</t>
         </is>
       </c>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>2.5 - 8.44</t>
+          <t>39 - 69</t>
         </is>
       </c>
       <c r="G15" s="1" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H15" s="1" t="inlineStr">
         <is>
-          <t>7/25/18</t>
+          <t>2/25/08</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>SWA-4-11</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>35.8736526</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>-106.3105976</t>
-        </is>
-      </c>
-      <c r="D16" s="1" t="inlineStr"/>
-      <c r="E16" s="1" t="inlineStr">
-        <is>
-          <t>9.17</t>
-        </is>
-      </c>
-      <c r="F16" s="1" t="inlineStr">
-        <is>
-          <t>3 - 9.17</t>
-        </is>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>44.4</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>8/15/17</t>
-        </is>
-      </c>
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Los Alamos and Pajarito Canyons</t>
+        </is>
+      </c>
+      <c r="H16" s="5" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>SWA-4-12</t>
+          <t>LAO-3a</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>35.8737001</t>
+          <t>35.87317</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>-106.3105616</t>
-        </is>
-      </c>
-      <c r="D17" s="1" t="inlineStr"/>
+          <t>-106.25822</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>9/14/89</t>
+        </is>
+      </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>8.53</t>
+          <t>14.7</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>2.99 - 8.19</t>
+          <t>4.7 - 14.7</t>
         </is>
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>56.2</t>
+          <t>13.9</t>
         </is>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
-          <t>8/15/17</t>
+          <t>9/17/03</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>Mortendad Canyon</t>
-        </is>
-      </c>
-      <c r="H18" s="5" t="n"/>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>LAUZ-1</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>35.87787</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>-106.27357</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr"/>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>10.55</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>5.35 - 10.35</t>
+        </is>
+      </c>
+      <c r="G18" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H18" s="1" t="inlineStr">
+        <is>
+          <t>8/20/97</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>MCO-0.6</t>
+          <t>PAO-5n</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>35.86789</t>
+          <t>35.87326</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>-106.30545</t>
+          <t>-106.22011</t>
         </is>
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>2/25/99</t>
+          <t>3/24/98</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>15.28</t>
         </is>
       </c>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>1.05 - 3.05</t>
+          <t>7.43 - 12.43</t>
         </is>
       </c>
       <c r="G19" s="1" t="inlineStr">
         <is>
-          <t>662</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H19" s="1" t="inlineStr">
         <is>
-          <t>7/2/10</t>
+          <t>6/4/15</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="inlineStr">
-        <is>
-          <t>Mortendad Canyon</t>
-        </is>
-      </c>
-      <c r="H20" s="5" t="n"/>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>18-MW-18</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>35.83237</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>-106.25166</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>7/31/95</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>12.5 - 23</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>3/19/07</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>MCO-5</t>
+          <t>PCAO-8</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>35.86339</t>
+          <t>35.82722</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>-106.27683</t>
+          <t>-106.23837</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>10/1/60</t>
+          <t>6/2/08</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>21 - 46</t>
+          <t>9.7 - 19.7</t>
         </is>
       </c>
       <c r="G21" s="1" t="inlineStr">
         <is>
-          <t>5.76</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H21" s="1" t="inlineStr">
         <is>
-          <t>7/6/10</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>MCO-7</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t>35.86056</t>
-        </is>
-      </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t>-106.26991</t>
-        </is>
-      </c>
-      <c r="D22" s="1" t="inlineStr">
-        <is>
-          <t>10/1/60</t>
-        </is>
-      </c>
-      <c r="E22" s="1" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
-      </c>
-      <c r="F22" s="1" t="inlineStr">
-        <is>
-          <t>39 - 69</t>
-        </is>
-      </c>
-      <c r="G22" s="1" t="inlineStr">
-        <is>
-          <t>5.44</t>
-        </is>
-      </c>
-      <c r="H22" s="1" t="inlineStr">
-        <is>
-          <t>7/7/10</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="inlineStr">
-        <is>
-          <t>Mortendad Canyon</t>
-        </is>
-      </c>
-      <c r="H23" s="5" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>LAO-3a</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>35.87317</t>
-        </is>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t>-106.25822</t>
-        </is>
-      </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>9/14/89</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>14.7</t>
-        </is>
-      </c>
-      <c r="F24" s="1" t="inlineStr">
-        <is>
-          <t>4.7 - 14.7</t>
-        </is>
-      </c>
-      <c r="G24" s="1" t="inlineStr">
-        <is>
-          <t>13.9</t>
-        </is>
-      </c>
-      <c r="H24" s="1" t="inlineStr">
-        <is>
-          <t>9/17/03</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>LAUZ-1</t>
-        </is>
-      </c>
-      <c r="B25" s="1" t="inlineStr">
-        <is>
-          <t>35.87787</t>
-        </is>
-      </c>
-      <c r="C25" s="1" t="inlineStr">
-        <is>
-          <t>-106.27357</t>
-        </is>
-      </c>
-      <c r="D25" s="1" t="inlineStr"/>
-      <c r="E25" s="1" t="inlineStr">
-        <is>
-          <t>10.55</t>
-        </is>
-      </c>
-      <c r="F25" s="1" t="inlineStr">
-        <is>
-          <t>5.35 - 10.35</t>
-        </is>
-      </c>
-      <c r="G25" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="H25" s="1" t="inlineStr">
-        <is>
-          <t>11/13/01</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>PAO-5n</t>
-        </is>
-      </c>
-      <c r="B26" s="1" t="inlineStr">
-        <is>
-          <t>35.87326</t>
-        </is>
-      </c>
-      <c r="C26" s="1" t="inlineStr">
-        <is>
-          <t>-106.22011</t>
-        </is>
-      </c>
-      <c r="D26" s="1" t="inlineStr">
-        <is>
-          <t>3/24/98</t>
-        </is>
-      </c>
-      <c r="E26" s="1" t="inlineStr">
-        <is>
-          <t>15.28</t>
-        </is>
-      </c>
-      <c r="F26" s="1" t="inlineStr">
-        <is>
-          <t>7.43 - 12.43</t>
-        </is>
-      </c>
-      <c r="G26" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="H26" s="1" t="inlineStr">
-        <is>
-          <t>6/11/02</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>18-MW-18</t>
-        </is>
-      </c>
-      <c r="B27" s="1" t="inlineStr">
-        <is>
-          <t>35.83237</t>
-        </is>
-      </c>
-      <c r="C27" s="1" t="inlineStr">
-        <is>
-          <t>-106.25166</t>
-        </is>
-      </c>
-      <c r="D27" s="1" t="inlineStr">
-        <is>
-          <t>7/31/95</t>
-        </is>
-      </c>
-      <c r="E27" s="1" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="F27" s="1" t="inlineStr">
-        <is>
-          <t>12.5 - 23</t>
-        </is>
-      </c>
-      <c r="G27" s="1" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="H27" s="1" t="inlineStr">
-        <is>
-          <t>3/19/07</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>PCAO-8</t>
-        </is>
-      </c>
-      <c r="B28" s="1" t="inlineStr">
-        <is>
-          <t>35.82722</t>
-        </is>
-      </c>
-      <c r="C28" s="1" t="inlineStr">
-        <is>
-          <t>-106.23837</t>
-        </is>
-      </c>
-      <c r="D28" s="1" t="inlineStr">
-        <is>
-          <t>6/2/08</t>
-        </is>
-      </c>
-      <c r="E28" s="1" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="F28" s="1" t="inlineStr">
-        <is>
-          <t>9.7 - 19.7</t>
-        </is>
-      </c>
-      <c r="G28" s="1" t="inlineStr">
-        <is>
-          <t>3.01</t>
-        </is>
-      </c>
-      <c r="H28" s="1" t="inlineStr">
-        <is>
-          <t>6/8/10</t>
+          <t>6/24/08</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A16:H16"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Had to update data with complete dataset back to 1980 then reprocess.
</commit_message>
<xml_diff>
--- a/Tables/Alluvial.xlsx
+++ b/Tables/Alluvial.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1236,7 +1236,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-7</t>
+          <t>SWA-2-4</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -1246,126 +1246,110 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>35.87376</t>
+          <t>35.8745609</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>-106.31114</t>
+          <t>-106.3125236</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr"/>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>2016-06-27 00:00:00</t>
-        </is>
-      </c>
+      <c r="G7" s="1" t="inlineStr"/>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 in</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>0.6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr">
         <is>
-          <t>Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7</t>
-        </is>
-      </c>
-      <c r="M7" s="1" t="inlineStr"/>
-      <c r="N7" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
-      <c r="O7" s="1" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
+          <t>Formerly SCPZ-4, Formerly SCPZ-4, Formerly SCPZ-4</t>
+        </is>
+      </c>
+      <c r="M7" s="1" t="inlineStr">
+        <is>
+          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12447</t>
+        </is>
+      </c>
+      <c r="N7" s="1" t="inlineStr"/>
+      <c r="O7" s="1" t="inlineStr"/>
       <c r="P7" s="1" t="inlineStr">
         <is>
           <t>Sandia</t>
         </is>
       </c>
-      <c r="Q7" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="Q7" s="1" t="inlineStr"/>
       <c r="R7" s="1" t="inlineStr"/>
       <c r="S7" s="1" t="inlineStr">
         <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T7" s="1" t="inlineStr">
-        <is>
-          <t>Aquifer updated from MW</t>
-        </is>
-      </c>
+          <t>7226.48</t>
+        </is>
+      </c>
+      <c r="T7" s="1" t="inlineStr"/>
       <c r="U7" s="1" t="inlineStr">
         <is>
-          <t>Well Info</t>
+          <t>Monitoring Wells</t>
         </is>
       </c>
       <c r="V7" s="1" t="inlineStr">
         <is>
-          <t>34.3</t>
+          <t>16.9</t>
         </is>
       </c>
       <c r="W7" s="1" t="inlineStr">
         <is>
-          <t>2017-08-16</t>
+          <t>2017-08-15</t>
         </is>
       </c>
       <c r="X7" s="1" t="inlineStr">
         <is>
-          <t>18.2</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="Y7" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>2019-10-24</t>
         </is>
       </c>
       <c r="Z7" s="1" t="inlineStr">
         <is>
-          <t>0.508</t>
+          <t>0.641</t>
         </is>
       </c>
       <c r="AA7" s="1" t="inlineStr">
         <is>
-          <t>2017-08-16</t>
+          <t>2017-08-15</t>
         </is>
       </c>
       <c r="AB7" s="1" t="inlineStr">
         <is>
-          <t>0.186</t>
+          <t>0.265</t>
         </is>
       </c>
       <c r="AC7" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>2019-10-24</t>
         </is>
       </c>
       <c r="AD7" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE7" s="1" t="inlineStr">
@@ -1388,7 +1372,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-8</t>
+          <t>SWA-2-5</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1398,96 +1382,80 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>35.8738</t>
+          <t>35.874674</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>-106.31109</t>
+          <t>-106.3124817</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr"/>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>2016-06-27 00:00:00</t>
-        </is>
-      </c>
+      <c r="G8" s="1" t="inlineStr"/>
       <c r="H8" s="1" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>8.96</t>
         </is>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 in</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>8.96</t>
         </is>
       </c>
       <c r="L8" s="1" t="inlineStr">
         <is>
-          <t>Formerly SWA-3, Formerly SWA-3, Formerly SWA-3, Formerly SWA-3</t>
-        </is>
-      </c>
-      <c r="M8" s="1" t="inlineStr"/>
-      <c r="N8" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
-      <c r="O8" s="1" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
+          <t>Formerly SCPZ-5, Formerly SCPZ-5, Formerly SCPZ-5</t>
+        </is>
+      </c>
+      <c r="M8" s="1" t="inlineStr">
+        <is>
+          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12448</t>
+        </is>
+      </c>
+      <c r="N8" s="1" t="inlineStr"/>
+      <c r="O8" s="1" t="inlineStr"/>
       <c r="P8" s="1" t="inlineStr">
         <is>
           <t>Sandia</t>
         </is>
       </c>
-      <c r="Q8" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="Q8" s="1" t="inlineStr"/>
       <c r="R8" s="1" t="inlineStr"/>
       <c r="S8" s="1" t="inlineStr">
         <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T8" s="1" t="inlineStr">
-        <is>
-          <t>Aquifer updated from MW</t>
-        </is>
-      </c>
+          <t>7226.22</t>
+        </is>
+      </c>
+      <c r="T8" s="1" t="inlineStr"/>
       <c r="U8" s="1" t="inlineStr">
         <is>
-          <t>Well Info</t>
+          <t>Monitoring Wells</t>
         </is>
       </c>
       <c r="V8" s="1" t="inlineStr">
         <is>
-          <t>22.0</t>
+          <t>8.28</t>
         </is>
       </c>
       <c r="W8" s="1" t="inlineStr">
         <is>
-          <t>2018-05-31</t>
+          <t>2018-02-28</t>
         </is>
       </c>
       <c r="X8" s="1" t="inlineStr">
         <is>
-          <t>14.1</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="Y8" s="1" t="inlineStr">
@@ -1497,17 +1465,17 @@
       </c>
       <c r="Z8" s="1" t="inlineStr">
         <is>
-          <t>1.22</t>
+          <t>0.366</t>
         </is>
       </c>
       <c r="AA8" s="1" t="inlineStr">
         <is>
-          <t>2017-11-30</t>
+          <t>2017-08-15</t>
         </is>
       </c>
       <c r="AB8" s="1" t="inlineStr">
         <is>
-          <t>0.473</t>
+          <t>0.358</t>
         </is>
       </c>
       <c r="AC8" s="1" t="inlineStr">
@@ -1540,7 +1508,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-9</t>
+          <t>SWA-2-6</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
@@ -1550,126 +1518,110 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>35.87386</t>
+          <t>35.8747486</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>-106.31105</t>
+          <t>-106.3124341</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr"/>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>2016-07-05 00:00:00</t>
-        </is>
-      </c>
+      <c r="G9" s="1" t="inlineStr"/>
       <c r="H9" s="1" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>8.22</t>
         </is>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 in</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>3.12</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>8.22</t>
         </is>
       </c>
       <c r="L9" s="1" t="inlineStr">
         <is>
-          <t>Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9</t>
-        </is>
-      </c>
-      <c r="M9" s="1" t="inlineStr"/>
-      <c r="N9" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
-      <c r="O9" s="1" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
+          <t>Formerly SWA-2, Formerly SWA-2, Formerly SWA-2</t>
+        </is>
+      </c>
+      <c r="M9" s="1" t="inlineStr">
+        <is>
+          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12449</t>
+        </is>
+      </c>
+      <c r="N9" s="1" t="inlineStr"/>
+      <c r="O9" s="1" t="inlineStr"/>
       <c r="P9" s="1" t="inlineStr">
         <is>
           <t>Sandia</t>
         </is>
       </c>
-      <c r="Q9" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="Q9" s="1" t="inlineStr"/>
       <c r="R9" s="1" t="inlineStr"/>
       <c r="S9" s="1" t="inlineStr">
         <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T9" s="1" t="inlineStr">
-        <is>
-          <t>Aquifer updated from MW</t>
-        </is>
-      </c>
+          <t>7225.72</t>
+        </is>
+      </c>
+      <c r="T9" s="1" t="inlineStr"/>
       <c r="U9" s="1" t="inlineStr">
         <is>
-          <t>Well Info</t>
+          <t>Monitoring Wells</t>
         </is>
       </c>
       <c r="V9" s="1" t="inlineStr">
         <is>
-          <t>15.9</t>
+          <t>7.38</t>
         </is>
       </c>
       <c r="W9" s="1" t="inlineStr">
         <is>
-          <t>2018-07-25</t>
+          <t>2018-02-28</t>
         </is>
       </c>
       <c r="X9" s="1" t="inlineStr">
         <is>
-          <t>9.02</t>
+          <t>3.85</t>
         </is>
       </c>
       <c r="Y9" s="1" t="inlineStr">
         <is>
+          <t>2019-10-24</t>
+        </is>
+      </c>
+      <c r="Z9" s="1" t="inlineStr">
+        <is>
+          <t>0.384</t>
+        </is>
+      </c>
+      <c r="AA9" s="1" t="inlineStr">
+        <is>
           <t>2019-02-27</t>
         </is>
       </c>
-      <c r="Z9" s="1" t="inlineStr">
-        <is>
-          <t>0.317</t>
-        </is>
-      </c>
-      <c r="AA9" s="1" t="inlineStr">
-        <is>
-          <t>2017-08-16</t>
-        </is>
-      </c>
       <c r="AB9" s="1" t="inlineStr">
         <is>
-          <t>0.174</t>
+          <t>0.152</t>
         </is>
       </c>
       <c r="AC9" s="1" t="inlineStr">
         <is>
-          <t>2019-02-27</t>
+          <t>2019-10-24</t>
         </is>
       </c>
       <c r="AD9" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE9" s="1" t="inlineStr">
@@ -1677,11 +1629,7 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF9" s="1" t="inlineStr">
-        <is>
-          <t>Exceedance</t>
-        </is>
-      </c>
+      <c r="AF9" s="1" t="inlineStr"/>
       <c r="AG9" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -1692,7 +1640,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>MCO-0.6</t>
+          <t>SWA-3-7</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
@@ -1702,32 +1650,24 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>35.86789</t>
+          <t>35.87376</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>-106.30545</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="inlineStr">
-        <is>
-          <t>7188.280</t>
-        </is>
-      </c>
-      <c r="F10" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
+          <t>-106.31114</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr"/>
+      <c r="F10" s="1" t="inlineStr"/>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>1999-02-25 00:00:00</t>
+          <t>2016-06-27 00:00:00</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>3.10</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="I10" s="1" t="inlineStr">
@@ -1737,15 +1677,19 @@
       </c>
       <c r="J10" s="1" t="inlineStr">
         <is>
-          <t>1.05</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="K10" s="1" t="inlineStr">
         <is>
-          <t>3.050</t>
-        </is>
-      </c>
-      <c r="L10" s="1" t="inlineStr"/>
+          <t>3.1</t>
+        </is>
+      </c>
+      <c r="L10" s="1" t="inlineStr">
+        <is>
+          <t>Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7, Formerly SCPZ-7</t>
+        </is>
+      </c>
       <c r="M10" s="1" t="inlineStr"/>
       <c r="N10" s="1" t="inlineStr">
         <is>
@@ -1759,7 +1703,7 @@
       </c>
       <c r="P10" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Sandia</t>
         </is>
       </c>
       <c r="Q10" s="1" t="inlineStr">
@@ -1773,7 +1717,11 @@
           <t>[84]</t>
         </is>
       </c>
-      <c r="T10" s="1" t="inlineStr"/>
+      <c r="T10" s="1" t="inlineStr">
+        <is>
+          <t>Aquifer updated from MW</t>
+        </is>
+      </c>
       <c r="U10" s="1" t="inlineStr">
         <is>
           <t>Well Info</t>
@@ -1781,47 +1729,47 @@
       </c>
       <c r="V10" s="1" t="inlineStr">
         <is>
-          <t>662.0</t>
+          <t>34.3</t>
         </is>
       </c>
       <c r="W10" s="1" t="inlineStr">
         <is>
-          <t>2010-07-02</t>
+          <t>2017-08-16</t>
         </is>
       </c>
       <c r="X10" s="1" t="inlineStr">
         <is>
-          <t>3.09</t>
+          <t>18.2</t>
         </is>
       </c>
       <c r="Y10" s="1" t="inlineStr">
         <is>
-          <t>2016-05-19</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="Z10" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.508</t>
         </is>
       </c>
       <c r="AA10" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2017-08-16</t>
         </is>
       </c>
       <c r="AB10" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.186</t>
         </is>
       </c>
       <c r="AC10" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="AD10" s="1" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>9</t>
         </is>
       </c>
       <c r="AE10" s="1" t="inlineStr">
@@ -1844,7 +1792,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>MCO-5</t>
+          <t>SWA-3-8</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
@@ -1854,60 +1802,60 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>35.86339</t>
+          <t>35.8738</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>-106.27683</t>
-        </is>
-      </c>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>6875.66</t>
-        </is>
-      </c>
-      <c r="F11" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
+          <t>-106.31109</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr"/>
+      <c r="F11" s="1" t="inlineStr"/>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>1960-10-01 00:00:00</t>
+          <t>2016-06-27 00:00:00</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
-          <t>46.00</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr">
         <is>
-          <t>46.000</t>
-        </is>
-      </c>
-      <c r="L11" s="1" t="inlineStr"/>
+          <t>7.8</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>Formerly SWA-3, Formerly SWA-3, Formerly SWA-3, Formerly SWA-3</t>
+        </is>
+      </c>
       <c r="M11" s="1" t="inlineStr"/>
-      <c r="N11" s="1" t="inlineStr"/>
+      <c r="N11" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
       <c r="O11" s="1" t="inlineStr">
         <is>
-          <t>Chromium</t>
+          <t>General</t>
         </is>
       </c>
       <c r="P11" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Sandia</t>
         </is>
       </c>
       <c r="Q11" s="1" t="inlineStr">
@@ -1923,7 +1871,7 @@
       </c>
       <c r="T11" s="1" t="inlineStr">
         <is>
-          <t>Ground Elevation updated from MW</t>
+          <t>Aquifer updated from MW</t>
         </is>
       </c>
       <c r="U11" s="1" t="inlineStr">
@@ -1933,47 +1881,47 @@
       </c>
       <c r="V11" s="1" t="inlineStr">
         <is>
-          <t>5.76</t>
+          <t>22.0</t>
         </is>
       </c>
       <c r="W11" s="1" t="inlineStr">
         <is>
-          <t>2010-07-06</t>
+          <t>2018-05-31</t>
         </is>
       </c>
       <c r="X11" s="1" t="inlineStr">
         <is>
-          <t>5.76</t>
+          <t>14.1</t>
         </is>
       </c>
       <c r="Y11" s="1" t="inlineStr">
         <is>
-          <t>2010-07-06</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="Z11" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>1.22</t>
         </is>
       </c>
       <c r="AA11" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2017-11-30</t>
         </is>
       </c>
       <c r="AB11" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.473</t>
         </is>
       </c>
       <c r="AC11" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="AD11" s="1" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE11" s="1" t="inlineStr">
@@ -1981,7 +1929,11 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF11" s="1" t="inlineStr"/>
+      <c r="AF11" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
       <c r="AG11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -1992,7 +1944,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>MCO-7</t>
+          <t>SWA-3-9</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
@@ -2002,60 +1954,60 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>35.86056</t>
+          <t>35.87386</t>
         </is>
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>-106.26991</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="inlineStr">
-        <is>
-          <t>6827.31</t>
-        </is>
-      </c>
-      <c r="F12" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
+          <t>-106.31105</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr"/>
+      <c r="F12" s="1" t="inlineStr"/>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>1960-10-01 00:00:00</t>
+          <t>2016-07-05 00:00:00</t>
         </is>
       </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
-          <t>69.00</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J12" s="1" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="K12" s="1" t="inlineStr">
         <is>
-          <t>69.000</t>
-        </is>
-      </c>
-      <c r="L12" s="1" t="inlineStr"/>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9, Formerly SCPZ-9</t>
+        </is>
+      </c>
       <c r="M12" s="1" t="inlineStr"/>
-      <c r="N12" s="1" t="inlineStr"/>
+      <c r="N12" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
       <c r="O12" s="1" t="inlineStr">
         <is>
-          <t>Chromium</t>
+          <t>General</t>
         </is>
       </c>
       <c r="P12" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Sandia</t>
         </is>
       </c>
       <c r="Q12" s="1" t="inlineStr">
@@ -2071,7 +2023,7 @@
       </c>
       <c r="T12" s="1" t="inlineStr">
         <is>
-          <t>Ground Elevation updated from MW</t>
+          <t>Aquifer updated from MW</t>
         </is>
       </c>
       <c r="U12" s="1" t="inlineStr">
@@ -2081,47 +2033,47 @@
       </c>
       <c r="V12" s="1" t="inlineStr">
         <is>
-          <t>5.44</t>
+          <t>15.9</t>
         </is>
       </c>
       <c r="W12" s="1" t="inlineStr">
         <is>
-          <t>2010-07-07</t>
+          <t>2018-07-25</t>
         </is>
       </c>
       <c r="X12" s="1" t="inlineStr">
         <is>
-          <t>5.44</t>
+          <t>9.02</t>
         </is>
       </c>
       <c r="Y12" s="1" t="inlineStr">
         <is>
-          <t>2010-07-07</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="Z12" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.317</t>
         </is>
       </c>
       <c r="AA12" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2017-08-16</t>
         </is>
       </c>
       <c r="AB12" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.174</t>
         </is>
       </c>
       <c r="AC12" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2019-02-27</t>
         </is>
       </c>
       <c r="AD12" s="1" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>9</t>
         </is>
       </c>
       <c r="AE12" s="1" t="inlineStr">
@@ -2129,7 +2081,11 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF12" s="1" t="inlineStr"/>
+      <c r="AF12" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
       <c r="AG12" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -2140,7 +2096,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>LAO-3a</t>
+          <t>SWA-4-10</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
@@ -2150,130 +2106,110 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>35.87317</t>
+          <t>35.8735723</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>-106.25822</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>6609.1</t>
-        </is>
-      </c>
-      <c r="F13" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
-      <c r="G13" s="1" t="inlineStr">
-        <is>
-          <t>1989-09-14 00:00:00</t>
-        </is>
-      </c>
+          <t>-106.3106197</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr"/>
+      <c r="F13" s="1" t="inlineStr"/>
+      <c r="G13" s="1" t="inlineStr"/>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>14.70</t>
+          <t>8.44</t>
         </is>
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 in</t>
         </is>
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr">
         <is>
-          <t>14.700</t>
+          <t>8.44</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
         <is>
-          <t>Elevation revised based on LIDAR surface location pick, Elevation revised based on LIDAR surface location pick</t>
-        </is>
-      </c>
-      <c r="M13" s="1" t="inlineStr"/>
+          <t>Formerly SCPZ-10, Formerly SCPZ-10, Formerly SCPZ-10</t>
+        </is>
+      </c>
+      <c r="M13" s="1" t="inlineStr">
+        <is>
+          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12453</t>
+        </is>
+      </c>
       <c r="N13" s="1" t="inlineStr"/>
-      <c r="O13" s="1" t="inlineStr">
-        <is>
-          <t>TA-21</t>
-        </is>
-      </c>
+      <c r="O13" s="1" t="inlineStr"/>
       <c r="P13" s="1" t="inlineStr">
         <is>
-          <t>Los Alamos</t>
-        </is>
-      </c>
-      <c r="Q13" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+          <t>Sandia</t>
+        </is>
+      </c>
+      <c r="Q13" s="1" t="inlineStr"/>
       <c r="R13" s="1" t="inlineStr"/>
       <c r="S13" s="1" t="inlineStr">
         <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T13" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
+          <t>7213.06</t>
+        </is>
+      </c>
+      <c r="T13" s="1" t="inlineStr"/>
       <c r="U13" s="1" t="inlineStr">
         <is>
-          <t>Well Info</t>
+          <t>Monitoring Wells</t>
         </is>
       </c>
       <c r="V13" s="1" t="inlineStr">
         <is>
-          <t>13.9</t>
+          <t>72.0</t>
         </is>
       </c>
       <c r="W13" s="1" t="inlineStr">
         <is>
-          <t>2003-09-17</t>
+          <t>2018-07-25</t>
         </is>
       </c>
       <c r="X13" s="1" t="inlineStr">
         <is>
-          <t>3.43</t>
+          <t>36.5</t>
         </is>
       </c>
       <c r="Y13" s="1" t="inlineStr">
         <is>
-          <t>2018-06-18</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="Z13" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="AA13" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2017-05-23</t>
         </is>
       </c>
       <c r="AB13" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.584</t>
         </is>
       </c>
       <c r="AC13" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="AD13" s="1" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE13" s="1" t="inlineStr">
@@ -2296,7 +2232,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>LAUZ-1</t>
+          <t>SWA-4-11</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -2306,122 +2242,110 @@
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>35.87787</t>
+          <t>35.8736526</t>
         </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>-106.27357</t>
-        </is>
-      </c>
-      <c r="E14" s="1" t="inlineStr">
-        <is>
-          <t>7032.42</t>
-        </is>
-      </c>
+          <t>-106.3105976</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr"/>
       <c r="G14" s="1" t="inlineStr"/>
       <c r="H14" s="1" t="inlineStr">
         <is>
-          <t>10.55</t>
+          <t>9.17</t>
         </is>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>4 in</t>
+          <t>2 in</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>5.35</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
         <is>
-          <t>10.350</t>
+          <t>9.17</t>
         </is>
       </c>
       <c r="L14" s="1" t="inlineStr">
         <is>
-          <t>DP Canyon, OU 1106 (TA-21), Surv-Tek Survey, Surv-Tek Survey</t>
-        </is>
-      </c>
-      <c r="M14" s="1" t="inlineStr"/>
+          <t>Formerly SCPZ-11(B), Formerly SCPZ-11(B), Formerly SCPZ-11(B)</t>
+        </is>
+      </c>
+      <c r="M14" s="1" t="inlineStr">
+        <is>
+          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12454</t>
+        </is>
+      </c>
       <c r="N14" s="1" t="inlineStr"/>
-      <c r="O14" s="1" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
+      <c r="O14" s="1" t="inlineStr"/>
       <c r="P14" s="1" t="inlineStr">
         <is>
-          <t>Los Alamos</t>
-        </is>
-      </c>
-      <c r="Q14" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+          <t>Sandia</t>
+        </is>
+      </c>
+      <c r="Q14" s="1" t="inlineStr"/>
       <c r="R14" s="1" t="inlineStr"/>
       <c r="S14" s="1" t="inlineStr">
         <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T14" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW, Well Diameter [in] updated from MW</t>
-        </is>
-      </c>
+          <t>7214.07</t>
+        </is>
+      </c>
+      <c r="T14" s="1" t="inlineStr"/>
       <c r="U14" s="1" t="inlineStr">
         <is>
-          <t>Well Info</t>
+          <t>Monitoring Wells</t>
         </is>
       </c>
       <c r="V14" s="1" t="inlineStr">
         <is>
-          <t>2.54</t>
+          <t>44.4</t>
         </is>
       </c>
       <c r="W14" s="1" t="inlineStr">
         <is>
-          <t>2001-11-13</t>
+          <t>2017-08-15</t>
         </is>
       </c>
       <c r="X14" s="1" t="inlineStr">
         <is>
-          <t>0.692</t>
+          <t>14.5</t>
         </is>
       </c>
       <c r="Y14" s="1" t="inlineStr">
         <is>
-          <t>2002-05-22</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="Z14" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>1.21</t>
         </is>
       </c>
       <c r="AA14" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2017-05-23</t>
         </is>
       </c>
       <c r="AB14" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.328</t>
         </is>
       </c>
       <c r="AC14" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="AD14" s="1" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE14" s="1" t="inlineStr">
@@ -2429,7 +2353,11 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF14" s="1" t="inlineStr"/>
+      <c r="AF14" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
       <c r="AG14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -2440,7 +2368,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>PAO-5n</t>
+          <t>SWA-4-12</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
@@ -2450,126 +2378,110 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>35.87326</t>
+          <t>35.8737001</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>-106.22011</t>
-        </is>
-      </c>
-      <c r="E15" s="1" t="inlineStr">
-        <is>
-          <t>6369.79</t>
-        </is>
-      </c>
-      <c r="F15" s="1" t="inlineStr">
-        <is>
-          <t>Qal</t>
-        </is>
-      </c>
-      <c r="G15" s="1" t="inlineStr">
-        <is>
-          <t>1998-03-24 00:00:00</t>
-        </is>
-      </c>
+          <t>-106.3105616</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="inlineStr"/>
+      <c r="F15" s="1" t="inlineStr"/>
+      <c r="G15" s="1" t="inlineStr"/>
       <c r="H15" s="1" t="inlineStr">
         <is>
-          <t>15.28</t>
+          <t>8.53</t>
         </is>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2 in</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>7.43</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
         <is>
-          <t>12.430</t>
-        </is>
-      </c>
-      <c r="L15" s="1" t="inlineStr"/>
-      <c r="M15" s="1" t="inlineStr"/>
+          <t>8.19</t>
+        </is>
+      </c>
+      <c r="L15" s="1" t="inlineStr">
+        <is>
+          <t>Formerly SWA-4, Formerly SWA-4, Formerly SWA-4</t>
+        </is>
+      </c>
+      <c r="M15" s="1" t="inlineStr">
+        <is>
+          <t>https://www.intellusnm.com/documents/document-library.cfc?method=retrieveLanlFile&amp;nodeId=12455</t>
+        </is>
+      </c>
       <c r="N15" s="1" t="inlineStr"/>
-      <c r="O15" s="1" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
+      <c r="O15" s="1" t="inlineStr"/>
       <c r="P15" s="1" t="inlineStr">
         <is>
-          <t>Los Alamos</t>
-        </is>
-      </c>
-      <c r="Q15" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+          <t>Sandia</t>
+        </is>
+      </c>
+      <c r="Q15" s="1" t="inlineStr"/>
       <c r="R15" s="1" t="inlineStr"/>
       <c r="S15" s="1" t="inlineStr">
         <is>
-          <t>[84]</t>
-        </is>
-      </c>
-      <c r="T15" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
+          <t>7213.04</t>
+        </is>
+      </c>
+      <c r="T15" s="1" t="inlineStr"/>
       <c r="U15" s="1" t="inlineStr">
         <is>
-          <t>Well Info</t>
+          <t>Monitoring Wells</t>
         </is>
       </c>
       <c r="V15" s="1" t="inlineStr">
         <is>
-          <t>No Detect Data</t>
+          <t>56.2</t>
         </is>
       </c>
       <c r="W15" s="1" t="inlineStr">
         <is>
-          <t>No Detect Data</t>
+          <t>2017-08-15</t>
         </is>
       </c>
       <c r="X15" s="1" t="inlineStr">
         <is>
-          <t>No Detect Data</t>
+          <t>31.8</t>
         </is>
       </c>
       <c r="Y15" s="1" t="inlineStr">
         <is>
-          <t>No Detect Data</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="Z15" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>1.74</t>
         </is>
       </c>
       <c r="AA15" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2017-05-23</t>
         </is>
       </c>
       <c r="AB15" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>0.693</t>
         </is>
       </c>
       <c r="AC15" s="1" t="inlineStr">
         <is>
-          <t>No Data</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="AD15" s="1" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE15" s="1" t="inlineStr">
@@ -2577,7 +2489,11 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="AF15" s="1" t="inlineStr"/>
+      <c r="AF15" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
       <c r="AG15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
@@ -2588,7 +2504,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>18-MW-18</t>
+          <t>MCO-0.6</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
@@ -2598,17 +2514,17 @@
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>35.83237</t>
+          <t>35.86789</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>-106.25166</t>
+          <t>-106.30545</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>6654.7</t>
+          <t>7188.280</t>
         </is>
       </c>
       <c r="F16" s="1" t="inlineStr">
@@ -2618,12 +2534,12 @@
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>1995-07-31 00:00:00</t>
+          <t>1999-02-25 00:00:00</t>
         </is>
       </c>
       <c r="H16" s="1" t="inlineStr">
         <is>
-          <t>23.00</t>
+          <t>3.10</t>
         </is>
       </c>
       <c r="I16" s="1" t="inlineStr">
@@ -2633,29 +2549,29 @@
       </c>
       <c r="J16" s="1" t="inlineStr">
         <is>
-          <t>12.5</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="K16" s="1" t="inlineStr">
         <is>
-          <t>23.000</t>
-        </is>
-      </c>
-      <c r="L16" s="1" t="inlineStr">
-        <is>
-          <t>TA-18</t>
-        </is>
-      </c>
+          <t>3.050</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr"/>
       <c r="M16" s="1" t="inlineStr"/>
-      <c r="N16" s="1" t="inlineStr"/>
+      <c r="N16" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
       <c r="O16" s="1" t="inlineStr">
         <is>
-          <t>TA-54</t>
+          <t>General</t>
         </is>
       </c>
       <c r="P16" s="1" t="inlineStr">
         <is>
-          <t>Pajarito</t>
+          <t>Mortendad</t>
         </is>
       </c>
       <c r="Q16" s="1" t="inlineStr">
@@ -2669,11 +2585,7 @@
           <t>[84]</t>
         </is>
       </c>
-      <c r="T16" s="1" t="inlineStr">
-        <is>
-          <t>Ground Elevation updated from MW</t>
-        </is>
-      </c>
+      <c r="T16" s="1" t="inlineStr"/>
       <c r="U16" s="1" t="inlineStr">
         <is>
           <t>Well Info</t>
@@ -2681,22 +2593,22 @@
       </c>
       <c r="V16" s="1" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>662.0</t>
         </is>
       </c>
       <c r="W16" s="1" t="inlineStr">
         <is>
-          <t>2007-03-19</t>
+          <t>2010-07-02</t>
         </is>
       </c>
       <c r="X16" s="1" t="inlineStr">
         <is>
-          <t>7.76</t>
+          <t>3.09</t>
         </is>
       </c>
       <c r="Y16" s="1" t="inlineStr">
         <is>
-          <t>2010-07-26</t>
+          <t>2016-05-19</t>
         </is>
       </c>
       <c r="Z16" s="1" t="inlineStr">
@@ -2721,7 +2633,7 @@
       </c>
       <c r="AD16" s="1" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>25</t>
         </is>
       </c>
       <c r="AE16" s="1" t="inlineStr">
@@ -2744,7 +2656,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>PCAO-8</t>
+          <t>MCO-5</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
@@ -2754,17 +2666,17 @@
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>35.82722</t>
+          <t>35.86339</t>
         </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>-106.23837</t>
+          <t>-106.27683</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>6584.450</t>
+          <t>6875.66</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
@@ -2774,48 +2686,40 @@
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>2008-06-02 00:00:00</t>
+          <t>1960-10-01 00:00:00</t>
         </is>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
-          <t>25.00</t>
+          <t>46.00</t>
         </is>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>21</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
         <is>
-          <t>19.700</t>
-        </is>
-      </c>
-      <c r="L17" s="1" t="inlineStr">
-        <is>
-          <t>Brass Cap, Brass Cap, Brass Cap</t>
-        </is>
-      </c>
+          <t>46.000</t>
+        </is>
+      </c>
+      <c r="L17" s="1" t="inlineStr"/>
       <c r="M17" s="1" t="inlineStr"/>
-      <c r="N17" s="1" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
+      <c r="N17" s="1" t="inlineStr"/>
       <c r="O17" s="1" t="inlineStr">
         <is>
-          <t>TA-54</t>
+          <t>Chromium</t>
         </is>
       </c>
       <c r="P17" s="1" t="inlineStr">
         <is>
-          <t>Pajarito</t>
+          <t>Mortendad</t>
         </is>
       </c>
       <c r="Q17" s="1" t="inlineStr">
@@ -2829,7 +2733,11 @@
           <t>[84]</t>
         </is>
       </c>
-      <c r="T17" s="1" t="inlineStr"/>
+      <c r="T17" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
       <c r="U17" s="1" t="inlineStr">
         <is>
           <t>Well Info</t>
@@ -2837,22 +2745,22 @@
       </c>
       <c r="V17" s="1" t="inlineStr">
         <is>
-          <t>3.01</t>
+          <t>5.76</t>
         </is>
       </c>
       <c r="W17" s="1" t="inlineStr">
         <is>
-          <t>2010-06-08</t>
+          <t>2010-07-06</t>
         </is>
       </c>
       <c r="X17" s="1" t="inlineStr">
         <is>
-          <t>3.01</t>
+          <t>5.76</t>
         </is>
       </c>
       <c r="Y17" s="1" t="inlineStr">
         <is>
-          <t>2010-06-08</t>
+          <t>2010-07-06</t>
         </is>
       </c>
       <c r="Z17" s="1" t="inlineStr">
@@ -2877,7 +2785,7 @@
       </c>
       <c r="AD17" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>52</t>
         </is>
       </c>
       <c r="AE17" s="1" t="inlineStr">
@@ -2887,6 +2795,914 @@
       </c>
       <c r="AF17" s="1" t="inlineStr"/>
       <c r="AG17" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Substantial
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>MCO-7</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>Alluvial</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>35.86056</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>-106.26991</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>6827.31</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
+      <c r="G18" s="1" t="inlineStr">
+        <is>
+          <t>1960-10-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="H18" s="1" t="inlineStr">
+        <is>
+          <t>69.00</t>
+        </is>
+      </c>
+      <c r="I18" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J18" s="1" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="K18" s="1" t="inlineStr">
+        <is>
+          <t>69.000</t>
+        </is>
+      </c>
+      <c r="L18" s="1" t="inlineStr"/>
+      <c r="M18" s="1" t="inlineStr"/>
+      <c r="N18" s="1" t="inlineStr"/>
+      <c r="O18" s="1" t="inlineStr">
+        <is>
+          <t>Chromium</t>
+        </is>
+      </c>
+      <c r="P18" s="1" t="inlineStr">
+        <is>
+          <t>Mortendad</t>
+        </is>
+      </c>
+      <c r="Q18" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R18" s="1" t="inlineStr"/>
+      <c r="S18" s="1" t="inlineStr">
+        <is>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T18" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
+      <c r="U18" s="1" t="inlineStr">
+        <is>
+          <t>Well Info</t>
+        </is>
+      </c>
+      <c r="V18" s="1" t="inlineStr">
+        <is>
+          <t>5.44</t>
+        </is>
+      </c>
+      <c r="W18" s="1" t="inlineStr">
+        <is>
+          <t>2010-07-07</t>
+        </is>
+      </c>
+      <c r="X18" s="1" t="inlineStr">
+        <is>
+          <t>5.44</t>
+        </is>
+      </c>
+      <c r="Y18" s="1" t="inlineStr">
+        <is>
+          <t>2010-07-07</t>
+        </is>
+      </c>
+      <c r="Z18" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AA18" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AB18" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AC18" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AD18" s="1" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="AE18" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="AF18" s="1" t="inlineStr"/>
+      <c r="AG18" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Substantial
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>LAO-3a</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>Alluvial</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>35.87317</t>
+        </is>
+      </c>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>-106.25822</t>
+        </is>
+      </c>
+      <c r="E19" s="1" t="inlineStr">
+        <is>
+          <t>6609.1</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
+      <c r="G19" s="1" t="inlineStr">
+        <is>
+          <t>1989-09-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="H19" s="1" t="inlineStr">
+        <is>
+          <t>14.70</t>
+        </is>
+      </c>
+      <c r="I19" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J19" s="1" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="K19" s="1" t="inlineStr">
+        <is>
+          <t>14.700</t>
+        </is>
+      </c>
+      <c r="L19" s="1" t="inlineStr">
+        <is>
+          <t>Elevation revised based on LIDAR surface location pick, Elevation revised based on LIDAR surface location pick</t>
+        </is>
+      </c>
+      <c r="M19" s="1" t="inlineStr"/>
+      <c r="N19" s="1" t="inlineStr"/>
+      <c r="O19" s="1" t="inlineStr">
+        <is>
+          <t>TA-21</t>
+        </is>
+      </c>
+      <c r="P19" s="1" t="inlineStr">
+        <is>
+          <t>Los Alamos</t>
+        </is>
+      </c>
+      <c r="Q19" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R19" s="1" t="inlineStr"/>
+      <c r="S19" s="1" t="inlineStr">
+        <is>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T19" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
+      <c r="U19" s="1" t="inlineStr">
+        <is>
+          <t>Well Info</t>
+        </is>
+      </c>
+      <c r="V19" s="1" t="inlineStr">
+        <is>
+          <t>13.9</t>
+        </is>
+      </c>
+      <c r="W19" s="1" t="inlineStr">
+        <is>
+          <t>2003-09-17</t>
+        </is>
+      </c>
+      <c r="X19" s="1" t="inlineStr">
+        <is>
+          <t>3.43</t>
+        </is>
+      </c>
+      <c r="Y19" s="1" t="inlineStr">
+        <is>
+          <t>2018-06-18</t>
+        </is>
+      </c>
+      <c r="Z19" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AA19" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AB19" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AC19" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AD19" s="1" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="AE19" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="AF19" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
+      <c r="AG19" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Substantial
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>LAUZ-1</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Alluvial</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>35.87787</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>-106.27357</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>7032.42</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr"/>
+      <c r="G20" s="1" t="inlineStr"/>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>10.55</t>
+        </is>
+      </c>
+      <c r="I20" s="1" t="inlineStr">
+        <is>
+          <t>4 in</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>5.35</t>
+        </is>
+      </c>
+      <c r="K20" s="1" t="inlineStr">
+        <is>
+          <t>10.350</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="inlineStr">
+        <is>
+          <t>DP Canyon, OU 1106 (TA-21), Surv-Tek Survey, Surv-Tek Survey</t>
+        </is>
+      </c>
+      <c r="M20" s="1" t="inlineStr"/>
+      <c r="N20" s="1" t="inlineStr"/>
+      <c r="O20" s="1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="P20" s="1" t="inlineStr">
+        <is>
+          <t>Los Alamos</t>
+        </is>
+      </c>
+      <c r="Q20" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R20" s="1" t="inlineStr"/>
+      <c r="S20" s="1" t="inlineStr">
+        <is>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T20" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW, Well Diameter [in] updated from MW</t>
+        </is>
+      </c>
+      <c r="U20" s="1" t="inlineStr">
+        <is>
+          <t>Well Info</t>
+        </is>
+      </c>
+      <c r="V20" s="1" t="inlineStr">
+        <is>
+          <t>28.9</t>
+        </is>
+      </c>
+      <c r="W20" s="1" t="inlineStr">
+        <is>
+          <t>1995-06-21</t>
+        </is>
+      </c>
+      <c r="X20" s="1" t="inlineStr">
+        <is>
+          <t>0.692</t>
+        </is>
+      </c>
+      <c r="Y20" s="1" t="inlineStr">
+        <is>
+          <t>2002-05-22</t>
+        </is>
+      </c>
+      <c r="Z20" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AA20" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AB20" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AC20" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AD20" s="1" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="AE20" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="AF20" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
+      <c r="AG20" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Substantial
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>PAO-5n</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>Alluvial</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>35.87326</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>-106.22011</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>6369.79</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="inlineStr">
+        <is>
+          <t>1998-03-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="H21" s="1" t="inlineStr">
+        <is>
+          <t>15.28</t>
+        </is>
+      </c>
+      <c r="I21" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J21" s="1" t="inlineStr">
+        <is>
+          <t>7.43</t>
+        </is>
+      </c>
+      <c r="K21" s="1" t="inlineStr">
+        <is>
+          <t>12.430</t>
+        </is>
+      </c>
+      <c r="L21" s="1" t="inlineStr"/>
+      <c r="M21" s="1" t="inlineStr"/>
+      <c r="N21" s="1" t="inlineStr"/>
+      <c r="O21" s="1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="P21" s="1" t="inlineStr">
+        <is>
+          <t>Los Alamos</t>
+        </is>
+      </c>
+      <c r="Q21" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R21" s="1" t="inlineStr"/>
+      <c r="S21" s="1" t="inlineStr">
+        <is>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T21" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
+      <c r="U21" s="1" t="inlineStr">
+        <is>
+          <t>Well Info</t>
+        </is>
+      </c>
+      <c r="V21" s="1" t="inlineStr">
+        <is>
+          <t>No Detect Data</t>
+        </is>
+      </c>
+      <c r="W21" s="1" t="inlineStr">
+        <is>
+          <t>No Detect Data</t>
+        </is>
+      </c>
+      <c r="X21" s="1" t="inlineStr">
+        <is>
+          <t>No Detect Data</t>
+        </is>
+      </c>
+      <c r="Y21" s="1" t="inlineStr">
+        <is>
+          <t>No Detect Data</t>
+        </is>
+      </c>
+      <c r="Z21" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AA21" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AB21" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AC21" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AD21" s="1" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="AE21" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="AF21" s="1" t="inlineStr"/>
+      <c r="AG21" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Substantial
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>18-MW-18</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>Alluvial</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>35.83237</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>-106.25166</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>6654.7</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>1995-07-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="H22" s="1" t="inlineStr">
+        <is>
+          <t>23.00</t>
+        </is>
+      </c>
+      <c r="I22" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J22" s="1" t="inlineStr">
+        <is>
+          <t>12.5</t>
+        </is>
+      </c>
+      <c r="K22" s="1" t="inlineStr">
+        <is>
+          <t>23.000</t>
+        </is>
+      </c>
+      <c r="L22" s="1" t="inlineStr">
+        <is>
+          <t>TA-18</t>
+        </is>
+      </c>
+      <c r="M22" s="1" t="inlineStr"/>
+      <c r="N22" s="1" t="inlineStr"/>
+      <c r="O22" s="1" t="inlineStr">
+        <is>
+          <t>TA-54</t>
+        </is>
+      </c>
+      <c r="P22" s="1" t="inlineStr">
+        <is>
+          <t>Pajarito</t>
+        </is>
+      </c>
+      <c r="Q22" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R22" s="1" t="inlineStr"/>
+      <c r="S22" s="1" t="inlineStr">
+        <is>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T22" s="1" t="inlineStr">
+        <is>
+          <t>Ground Elevation updated from MW</t>
+        </is>
+      </c>
+      <c r="U22" s="1" t="inlineStr">
+        <is>
+          <t>Well Info</t>
+        </is>
+      </c>
+      <c r="V22" s="1" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="W22" s="1" t="inlineStr">
+        <is>
+          <t>2007-03-19</t>
+        </is>
+      </c>
+      <c r="X22" s="1" t="inlineStr">
+        <is>
+          <t>7.76</t>
+        </is>
+      </c>
+      <c r="Y22" s="1" t="inlineStr">
+        <is>
+          <t>2010-07-26</t>
+        </is>
+      </c>
+      <c r="Z22" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AA22" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AB22" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AC22" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AD22" s="1" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="AE22" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="AF22" s="1" t="inlineStr">
+        <is>
+          <t>Exceedance</t>
+        </is>
+      </c>
+      <c r="AG22" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Substantial
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>PCAO-8</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>Alluvial</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>35.82722</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>-106.23837</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>6584.450</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>Qal</t>
+        </is>
+      </c>
+      <c r="G23" s="1" t="inlineStr">
+        <is>
+          <t>2008-06-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="H23" s="1" t="inlineStr">
+        <is>
+          <t>25.00</t>
+        </is>
+      </c>
+      <c r="I23" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J23" s="1" t="inlineStr">
+        <is>
+          <t>9.7</t>
+        </is>
+      </c>
+      <c r="K23" s="1" t="inlineStr">
+        <is>
+          <t>19.700</t>
+        </is>
+      </c>
+      <c r="L23" s="1" t="inlineStr">
+        <is>
+          <t>Brass Cap, Brass Cap, Brass Cap</t>
+        </is>
+      </c>
+      <c r="M23" s="1" t="inlineStr"/>
+      <c r="N23" s="1" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="O23" s="1" t="inlineStr">
+        <is>
+          <t>TA-54</t>
+        </is>
+      </c>
+      <c r="P23" s="1" t="inlineStr">
+        <is>
+          <t>Pajarito</t>
+        </is>
+      </c>
+      <c r="Q23" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R23" s="1" t="inlineStr"/>
+      <c r="S23" s="1" t="inlineStr">
+        <is>
+          <t>[84]</t>
+        </is>
+      </c>
+      <c r="T23" s="1" t="inlineStr"/>
+      <c r="U23" s="1" t="inlineStr">
+        <is>
+          <t>Well Info</t>
+        </is>
+      </c>
+      <c r="V23" s="1" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W23" s="1" t="inlineStr">
+        <is>
+          <t>2010-06-08</t>
+        </is>
+      </c>
+      <c r="X23" s="1" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="Y23" s="1" t="inlineStr">
+        <is>
+          <t>2010-06-08</t>
+        </is>
+      </c>
+      <c r="Z23" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AA23" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AB23" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AC23" s="1" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
+      </c>
+      <c r="AD23" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="AE23" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="AF23" s="1" t="inlineStr"/>
+      <c r="AG23" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Substantial
 </t>
@@ -2904,7 +3720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2912,12 +3728,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11.29"/>
+    <col customWidth="1" max="1" min="1" width="12.25"/>
     <col customWidth="1" max="2" min="2" width="10.14"/>
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="9.15"/>
     <col customWidth="1" max="5" min="5" width="7"/>
-    <col customWidth="1" max="6" min="6" width="13.43"/>
+    <col customWidth="1" max="6" min="6" width="16.25"/>
     <col customWidth="1" max="7" min="7" width="8.43"/>
     <col customWidth="1" max="8" min="8" width="8.43"/>
   </cols>
@@ -3160,472 +3976,700 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-7</t>
+          <t>SWA-2-4</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>35.87376</t>
+          <t>35.8745609</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>-106.31114</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>6/27/16</t>
-        </is>
-      </c>
+          <t>-106.3125236</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>0.6 - 3.1</t>
+          <t>3 - 9</t>
         </is>
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>34.3</t>
+          <t>16.9</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
-          <t>8/16/17</t>
+          <t>8/15/17</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-8</t>
+          <t>SWA-2-5</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>35.8738</t>
+          <t>35.874674</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>-106.31109</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>6/27/16</t>
-        </is>
-      </c>
+          <t>-106.3124817</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>8.96</t>
         </is>
       </c>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>3.6 - 7.8</t>
+          <t>3 - 8.96</t>
         </is>
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>8.28</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>5/31/18</t>
+          <t>2/28/18</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>SWA-3-9</t>
+          <t>SWA-2-6</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>35.87386</t>
+          <t>35.8747486</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>-106.31105</t>
-        </is>
-      </c>
-      <c r="D11" s="1" t="inlineStr">
-        <is>
-          <t>7/5/16</t>
-        </is>
-      </c>
+          <t>-106.3124341</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>8.22</t>
         </is>
       </c>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>2.2 - 4.7</t>
+          <t>3.12 - 8.22</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>15.9</t>
+          <t>7.38</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
-          <t>7/25/18</t>
+          <t>2/28/18</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Mortendad Canyon</t>
-        </is>
-      </c>
-      <c r="H12" s="5" t="n"/>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>SWA-3-7</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>35.87376</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>-106.31114</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>6/27/16</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>0.6 - 3.1</t>
+        </is>
+      </c>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>34.3</t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="inlineStr">
+        <is>
+          <t>8/16/17</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>MCO-0.6</t>
+          <t>SWA-3-8</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>35.86789</t>
+          <t>35.8738</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>-106.30545</t>
+          <t>-106.31109</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>2/25/99</t>
+          <t>6/27/16</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>1.05 - 3.05</t>
+          <t>3.6 - 7.8</t>
         </is>
       </c>
       <c r="G13" s="1" t="inlineStr">
         <is>
-          <t>662</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>7/2/10</t>
+          <t>5/31/18</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>MCO-5</t>
+          <t>SWA-3-9</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>35.86339</t>
+          <t>35.87386</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>-106.27683</t>
+          <t>-106.31105</t>
         </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>10/1/60</t>
+          <t>7/5/16</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>21 - 46</t>
+          <t>2.2 - 4.7</t>
         </is>
       </c>
       <c r="G14" s="1" t="inlineStr">
         <is>
-          <t>5.76</t>
+          <t>15.9</t>
         </is>
       </c>
       <c r="H14" s="1" t="inlineStr">
         <is>
-          <t>7/6/10</t>
+          <t>7/25/18</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>MCO-7</t>
+          <t>SWA-4-10</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>35.86056</t>
+          <t>35.8735723</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>-106.26991</t>
-        </is>
-      </c>
-      <c r="D15" s="1" t="inlineStr">
-        <is>
-          <t>10/1/60</t>
-        </is>
-      </c>
+          <t>-106.3106197</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>8.44</t>
         </is>
       </c>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>39 - 69</t>
+          <t>2.5 - 8.44</t>
         </is>
       </c>
       <c r="G15" s="1" t="inlineStr">
         <is>
-          <t>5.44</t>
+          <t>72</t>
         </is>
       </c>
       <c r="H15" s="1" t="inlineStr">
         <is>
-          <t>7/7/10</t>
+          <t>7/25/18</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>Los Alamos and Pajarito Canyons</t>
-        </is>
-      </c>
-      <c r="H16" s="5" t="n"/>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>SWA-4-11</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>35.8736526</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>-106.3105976</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr"/>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>9.17</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>3 - 9.17</t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>44.4</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>8/15/17</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>LAO-3a</t>
+          <t>SWA-4-12</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>35.87317</t>
+          <t>35.8737001</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>-106.25822</t>
-        </is>
-      </c>
-      <c r="D17" s="1" t="inlineStr">
-        <is>
-          <t>9/14/89</t>
-        </is>
-      </c>
+          <t>-106.3105616</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr"/>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>14.7</t>
+          <t>8.53</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>4.7 - 14.7</t>
+          <t>2.99 - 8.19</t>
         </is>
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>13.9</t>
+          <t>56.2</t>
         </is>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
-          <t>9/17/03</t>
+          <t>8/15/17</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>LAUZ-1</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>35.87787</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>-106.27357</t>
-        </is>
-      </c>
-      <c r="D18" s="1" t="inlineStr"/>
-      <c r="E18" s="1" t="inlineStr">
-        <is>
-          <t>10.55</t>
-        </is>
-      </c>
-      <c r="F18" s="1" t="inlineStr">
-        <is>
-          <t>5.35 - 10.35</t>
-        </is>
-      </c>
-      <c r="G18" s="1" t="inlineStr">
-        <is>
-          <t>2.54</t>
-        </is>
-      </c>
-      <c r="H18" s="1" t="inlineStr">
-        <is>
-          <t>11/13/01</t>
-        </is>
-      </c>
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Mortendad Canyon</t>
+        </is>
+      </c>
+      <c r="H18" s="5" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>PAO-5n</t>
+          <t>MCO-0.6</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>35.87326</t>
+          <t>35.86789</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>-106.22011</t>
+          <t>-106.30545</t>
         </is>
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>3/24/98</t>
+          <t>2/25/99</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>15.28</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>7.43 - 12.43</t>
+          <t>1.05 - 3.05</t>
         </is>
       </c>
       <c r="G19" s="1" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>662</t>
         </is>
       </c>
       <c r="H19" s="1" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>7/2/10</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>18-MW-18</t>
+          <t>MCO-5</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>35.83237</t>
+          <t>35.86339</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>-106.25166</t>
+          <t>-106.27683</t>
         </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>7/31/95</t>
+          <t>10/1/60</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>12.5 - 23</t>
+          <t>21 - 46</t>
         </is>
       </c>
       <c r="G20" s="1" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5.76</t>
         </is>
       </c>
       <c r="H20" s="1" t="inlineStr">
         <is>
-          <t>3/19/07</t>
+          <t>7/6/10</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
+          <t>MCO-7</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>35.86056</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>-106.26991</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>10/1/60</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>39 - 69</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="inlineStr">
+        <is>
+          <t>5.44</t>
+        </is>
+      </c>
+      <c r="H21" s="1" t="inlineStr">
+        <is>
+          <t>7/7/10</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>Los Alamos and Pajarito Canyons</t>
+        </is>
+      </c>
+      <c r="H22" s="5" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>LAO-3a</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>35.87317</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>-106.25822</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>9/14/89</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>14.7</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>4.7 - 14.7</t>
+        </is>
+      </c>
+      <c r="G23" s="1" t="inlineStr">
+        <is>
+          <t>13.9</t>
+        </is>
+      </c>
+      <c r="H23" s="1" t="inlineStr">
+        <is>
+          <t>9/17/03</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>LAUZ-1</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>35.87787</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>-106.27357</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr"/>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>10.55</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>5.35 - 10.35</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>28.9</t>
+        </is>
+      </c>
+      <c r="H24" s="1" t="inlineStr">
+        <is>
+          <t>6/21/95</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>PAO-5n</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>35.87326</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>-106.22011</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>3/24/98</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>15.28</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>7.43 - 12.43</t>
+        </is>
+      </c>
+      <c r="G25" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H25" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>18-MW-18</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>35.83237</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>-106.25166</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>7/31/95</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>12.5 - 23</t>
+        </is>
+      </c>
+      <c r="G26" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="H26" s="1" t="inlineStr">
+        <is>
+          <t>3/19/07</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
           <t>PCAO-8</t>
         </is>
       </c>
-      <c r="B21" s="1" t="inlineStr">
+      <c r="B27" s="1" t="inlineStr">
         <is>
           <t>35.82722</t>
         </is>
       </c>
-      <c r="C21" s="1" t="inlineStr">
+      <c r="C27" s="1" t="inlineStr">
         <is>
           <t>-106.23837</t>
         </is>
       </c>
-      <c r="D21" s="1" t="inlineStr">
+      <c r="D27" s="1" t="inlineStr">
         <is>
           <t>6/2/08</t>
         </is>
       </c>
-      <c r="E21" s="1" t="inlineStr">
+      <c r="E27" s="1" t="inlineStr">
         <is>
           <t>25</t>
         </is>
       </c>
-      <c r="F21" s="1" t="inlineStr">
+      <c r="F27" s="1" t="inlineStr">
         <is>
           <t>9.7 - 19.7</t>
         </is>
       </c>
-      <c r="G21" s="1" t="inlineStr">
+      <c r="G27" s="1" t="inlineStr">
         <is>
           <t>3.01</t>
         </is>
       </c>
-      <c r="H21" s="1" t="inlineStr">
+      <c r="H27" s="1" t="inlineStr">
         <is>
           <t>6/8/10</t>
         </is>
@@ -3635,8 +4679,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>